<commit_message>
pushing to share with group
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D943A2E7-7C25-9643-B7E6-DAF891BACCB7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7D3336-8345-EC47-BA03-7AA74123A540}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
@@ -223,45 +223,48 @@
 Topics: Core activities of Requirements Engineering, Characteristics of a Requirements Engineer, Types of Requirements Engineerings, Categorization;</t>
   </si>
   <si>
+    <t>Topic: name- Week 5,lectures- 2 Lectures, duration- 01:31;
+Video: link- https://drive.google.com/file/d/1oXdOllR8M09Fn_R6kxg6Na6fg9YhNBlG/preview, name- SRE Week#5Part1, duration- 00:41;
+Video: link- https://drive.google.com/file/d/155VGfcSrMOFxiFuPAVVUkFdSdLdVUH9o/preview, name- SRE Week#5Part2, duration- 00:50;
+Topics: Risk factors while selecting elicitation techniques, Human influences, Organzational influences, Operational influences, Combining elicitation techniques, Survey techniques, a. Eliciting explicit knowledge, b. Interview, c. Questionnaire, Creative Techniques, a. Brain Storming, b. Brain Storming Paradox, c. Change of percpective, d. Analogy, Documentcentric Techniques, a. System Archeology, b. Percpective Reading, c. Reuse, Observation Techniques, a. Question observations and optimize process, b.Field observation, c. Apprenticing, Support Techniques, a. Mind mapping, b. Workshops, c. CRC cards, d. Audio and Video recordings, e. Modelling action sequences, f. Prototypes for illustration;</t>
+  </si>
+  <si>
+    <t>Subject: Software Requirement Engineering;
+Instructor: Mr Adil Ahmed | +92 321 5185989;
+ClassSenior: Fakhar | +92 ‭332 0278998‬;
+Note: Most of the questions in papers will come from slides. If we prepare slides only we will make it.;
+CreditHours: 2.0;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 3,lectures- 1 Lecture, duration- 01:03;
+Video: link- https://drive.google.com/file/d/1f-_LejqI4_0bTJl9ld5vK7xt1ftYtFt5/preview, name- SRE Week#3, duration- 01:03;
+Slides: slide- Lecture Slide_2.pptx;
+Topics: System and Context Boundaries, Context aspects in the system context, Defining System Boundary, Defining the Context Boundary, Documenting the System Context;
+Quiz: name- Quiz 1,img- ,</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 4,lectures- 2 Lectures, duration- 01:06;
+Video: link- https://drive.google.com/file/d/1BmiDBx3Ve2JXQoaLMt2cid9n5IhCDzlK/preview, name- SRE Week#4Part1, duration- 00:57;
+Video: link- https://drive.google.com/file/d/1ZiBHNHotKvuJhOO9taLzR3gdPfy1DgVZ/preview, name- SRE Week#4Part2, duration- 00:09;
+Slides: slide- Lecture Slide_3.pptx;
+Topics: Eliciting Requirements Sources, Documenting Stakeholders, Obligations of requirements Engineer, Obligations of stakeholders, Kano Model, Categories of satisfaction, Satisfiers, Delighters, Dissatisfiers, Elicitation Techniques (Introduction), Influencing factors regarding the choice of elicitation techniques;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 6,lectures- 1 Lecture, duration- 01:07;
+Video: link- https://drive.google.com/file/d/14EjJ9UzO_AGydV_w9UJIKyfJJMjCwjlW/preview, name- SRE Week#6, duration- 01:07;
+Slides: slide- Lecture Slide_4.pptx;
+Topics: Document Design, Reasons for documentation, a. Central role of requirements, b. Legal relevance, c. Complexity, d. Accessibility, Types of Documentation, a. Data perspective, b. Functional perspective, c. Behaviourial perspective, Advantages of using natural language, Disadvantages of using natural language,  Requirements Documentation using Conceptual Models, a. Use case diagram, b. Structural data modeling and structuring of terms class diagram, c. Sequence modelling, d. State diagram, Hybrid Requirements Documents;</t>
+  </si>
+  <si>
     <t xml:space="preserve">Topic: name- Week 1,lectures- 3 Lectures, duration- 01:47;
 Video: link- https://drive.google.com/file/d/1brUQVmv6OGb2n1GePe4c5fjrVbVJUFvz/preview, name- Class CR Number, duration- 00:04;
 Video: link- https://drive.google.com/file/d/1-oeLFxAxdOeAgkILn1uyLbTcr-NsZlIT/preview, name- SRE Week#1 Part1.mp4, duration- 56:47;
 Video: link- https://drive.google.com/file/d/1niJ6P3J5h1XEUlyBzUgIHOfQzYw9hk1K/preview, name- SRE Week#1 Part2.mp4, duration- 51:36;
-Slides: Lecture Slide_1.pptx;Topics: Stakeholders, Goal of Requirements Engineering, Core activities of Requirements Engineering;
-Books: Requirements Engineering a good practice guide by Ian Sommervilla &amp; Pete Sawyer, Software Requirements 3rd Edtion by Xarl Wuuigers &amp; Joy Beatty, Engineering &amp; Managing Software REquirements by Ayubuke Aurum &amp; Class Wohlin; </t>
-  </si>
-  <si>
-    <t>Topic: name- Week 3,lectures- 1 Lecture, duration- 01:03;
-Video: link- https://drive.google.com/file/d/1f-_LejqI4_0bTJl9ld5vK7xt1ftYtFt5/preview, name- SRE Week#3, duration- 01:03;
-Slides: Lecture Slide_2.pptx;
-Topics: System and Context Boundaries, Context aspects in the system context, Defining System Boundary, Defining the Context Boundary, Documenting the System Context;
-Quiz: name- Quiz 1,img- ,</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 4,lectures- 2 Lectures, duration- 01:06;
-Video: link- https://drive.google.com/file/d/1BmiDBx3Ve2JXQoaLMt2cid9n5IhCDzlK/preview, name- SRE Week#4Part1, duration- 00:57;
-Video: link- https://drive.google.com/file/d/1ZiBHNHotKvuJhOO9taLzR3gdPfy1DgVZ/preview, name- SRE Week#4Part2, duration- 00:09;
-Slides: Lecture Slide_3.pptx;
-Topics: Eliciting Requirements Sources, Documenting Stakeholders, Obligations of requirements Engineer, Obligations of stakeholders, Kano Model, Categories of satisfaction, Satisfiers, Delighters, Dissatisfiers, Elicitation Techniques (Introduction), Influencing factors regarding the choice of elicitation techniques;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 5,lectures- 2 Lectures, duration- 01:31;
-Video: link- https://drive.google.com/file/d/1oXdOllR8M09Fn_R6kxg6Na6fg9YhNBlG/preview, name- SRE Week#5Part1, duration- 00:41;
-Video: link- https://drive.google.com/file/d/155VGfcSrMOFxiFuPAVVUkFdSdLdVUH9o/preview, name- SRE Week#5Part2, duration- 00:50;
-Topics: Risk factors while selecting elicitation techniques, Human influences, Organzational influences, Operational influences, Combining elicitation techniques, Survey techniques, a. Eliciting explicit knowledge, b. Interview, c. Questionnaire, Creative Techniques, a. Brain Storming, b. Brain Storming Paradox, c. Change of percpective, d. Analogy, Documentcentric Techniques, a. System Archeology, b. Percpective Reading, c. Reuse, Observation Techniques, a. Question observations and optimize process, b.Field observation, c. Apprenticing, Support Techniques, a. Mind mapping, b. Workshops, c. CRC cards, d. Audio and Video recordings, e. Modelling action sequences, f. Prototypes for illustration;</t>
-  </si>
-  <si>
-    <t>Subject: Software Requirement Engineering;
-Instructor: Mr Adil Ahmed, +92 321 5185989;
-Class Senior: Fakhar, +92 ‭332 0278998‬;
-Note: Most of the questions in papers will come from slides. If we prepare slides only we will make it.;
-Credit Hours: 2.0;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 6,lectures- 1 Lecture, duration- 01:07;
-Video: link- https://drive.google.com/file/d/14EjJ9UzO_AGydV_w9UJIKyfJJMjCwjlW/preview, name- SRE Week#6, duration- 01:07;
-Slides: Lecture Slide_4.pptx;
-Topics: Document Design, Reasons for documentation, a. Central role of requirements, b. Legal relevance, c. Complexity, d. Accessibility, Types of Documentation, a. Data perspective, b. Functional perspective, c. Behaviourial perspective, Advantages of using natural language, Disadvantages of using natural language,  Requirements Documentation using Conceptual Models, a. Use case diagram, b. Structural data modeling and structuring of terms class diagram, c. Sequence modelling, d. State diagram, Hybrid Requirements Documents;</t>
+Slides: slide- Lecture Slide_1.pptx;
+Topics: Stakeholders, Goal of Requirements Engineering, Core activities of Requirements Engineering;
+Books: name- Requirements Engineering a good practice guide by Ian Sommervilla &amp; Pete Sawyer;
+Books: name- Software Requirements 3rd Edtion by Xarl Wuuigers &amp; Joy Beatty;
+Books: name- Engineering &amp; Managing Software REquirements by Ayubuke Aurum &amp; Class Wohlin; </t>
   </si>
 </sst>
 </file>
@@ -678,7 +681,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB8366-CFB7-BD41-BAF1-2BC53FC93C19}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -721,7 +724,7 @@
         <v>29</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>30</v>
@@ -730,14 +733,14 @@
       <c r="G2" s="12"/>
       <c r="N2" s="6"/>
     </row>
-    <row r="3" spans="1:14" ht="306" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="340" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>43720</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="14"/>
       <c r="D3" s="14" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E3" s="14"/>
       <c r="F3" s="14"/>
@@ -765,7 +768,7 @@
       <c r="B5" s="8"/>
       <c r="C5" s="5"/>
       <c r="D5" s="14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E5" s="5"/>
       <c r="N5" s="5"/>
@@ -777,7 +780,7 @@
       <c r="B6" s="8"/>
       <c r="C6" s="5"/>
       <c r="D6" s="14" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E6" s="5"/>
       <c r="N6" s="5"/>
@@ -789,7 +792,7 @@
       <c r="B7" s="8"/>
       <c r="C7" s="5"/>
       <c r="D7" s="14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="10"/>
@@ -803,7 +806,7 @@
       <c r="B8" s="8"/>
       <c r="C8" s="5"/>
       <c r="D8" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="10"/>

</xml_diff>

<commit_message>
quiz pic test added
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0C4DF4-6605-F24C-8086-3A5470806625}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4A7289-D242-DD43-A2F7-9D995F290AC9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
@@ -215,24 +215,11 @@
 Topics: Risk factors while selecting elicitation techniques, Human influences, Organzational influences, Operational influences, Combining elicitation techniques, Survey techniques, a. Eliciting explicit knowledge, b. Interview, c. Questionnaire, Creative Techniques, a. Brain Storming, b. Brain Storming Paradox, c. Change of percpective, d. Analogy, Documentcentric Techniques, a. System Archeology, b. Percpective Reading, c. Reuse, Observation Techniques, a. Question observations and optimize process, b.Field observation, c. Apprenticing, Support Techniques, a. Mind mapping, b. Workshops, c. CRC cards, d. Audio and Video recordings, e. Modelling action sequences, f. Prototypes for illustration;</t>
   </si>
   <si>
-    <t>Topic: name- Week 3,lectures- 1 Lecture, duration- 01:03;
-Video: link- https://drive.google.com/file/d/1f-_LejqI4_0bTJl9ld5vK7xt1ftYtFt5/preview, name- SRE Week#3, duration- 01:03;
-Slides: slide- Lecture Slide_2.pptx;
-Topics: System and Context Boundaries, Context aspects in the system context, Defining System Boundary, Defining the Context Boundary, Documenting the System Context;
-Quiz: name- Quiz 1,img- ,</t>
-  </si>
-  <si>
     <t>Topic: name- Week 4,lectures- 2 Lectures, duration- 01:06;
 Video: link- https://drive.google.com/file/d/1BmiDBx3Ve2JXQoaLMt2cid9n5IhCDzlK/preview, name- SRE Week#4Part1, duration- 00:57;
 Video: link- https://drive.google.com/file/d/1ZiBHNHotKvuJhOO9taLzR3gdPfy1DgVZ/preview, name- SRE Week#4Part2, duration- 00:09;
 Slides: slide- Lecture Slide_3.pptx;
 Topics: Eliciting Requirements Sources, Documenting Stakeholders, Obligations of requirements Engineer, Obligations of stakeholders, Kano Model, Categories of satisfaction, Satisfiers, Delighters, Dissatisfiers, Elicitation Techniques (Introduction), Influencing factors regarding the choice of elicitation techniques;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 6,lectures- 1 Lecture, duration- 01:07;
-Video: link- https://drive.google.com/file/d/14EjJ9UzO_AGydV_w9UJIKyfJJMjCwjlW/preview, name- SRE Week#6, duration- 01:07;
-Slides: slide- Lecture Slide_4.pptx;
-Topics: Document Design, Reasons for documentation, a. Central role of requirements, b. Legal relevance, c. Complexity, d. Accessibility, Types of Documentation, a. Data perspective, b. Functional perspective, c. Behaviourial perspective, Advantages of using natural language, Disadvantages of using natural language,  Requirements Documentation using Conceptual Models, a. Use case diagram, b. Structural data modeling and structuring of terms class diagram, c. Sequence modelling, d. State diagram, Hybrid Requirements Documents;</t>
   </si>
   <si>
     <t>Topic: name- Week 1,lectures- 3 Lectures, duration- 01:47;
@@ -312,6 +299,20 @@
 ClassSenior: +92 301 3068788‬;
 Note: Not prepared all lectures, but most of the syllabus comes from slides.;
 CreditHours: 3.0;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 6,lectures- 1 Lecture, duration- 01:07;
+Video: link- https://drive.google.com/file/d/14EjJ9UzO_AGydV_w9UJIKyfJJMjCwjlW/preview, name- SRE Week#6, duration- 01:07;
+Slides: slide- Lecture Slide_4.pptx;
+Topics: Document Design, Reasons for documentation, a. Central role of requirements, b. Legal relevance, c. Complexity, d. Accessibility, Types of Documentation, a. Data perspective, b. Functional perspective, c. Behaviourial perspective, Advantages of using natural language, Disadvantages of using natural language,  Requirements Documentation using Conceptual Models, a. Use case diagram, b. Structural data modeling and structuring of terms class diagram, c. Sequence modelling, d. State diagram, Hybrid Requirements Documents;
+Quiz: name- Quiz 2;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 3,lectures- 1 Lecture, duration- 01:03;
+Video: link- https://drive.google.com/file/d/1f-_LejqI4_0bTJl9ld5vK7xt1ftYtFt5/preview, name- SRE Week#3, duration- 01:03;
+Slides: slide- Lecture Slide_2.pptx;
+Topics: System and Context Boundaries, Context aspects in the system context, Defining System Boundary, Defining the Context Boundary, Documenting the System Context;
+Quiz: name- Quiz 1;</t>
   </si>
 </sst>
 </file>
@@ -728,8 +729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB8366-CFB7-BD41-BAF1-2BC53FC93C19}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -768,13 +769,13 @@
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="12"/>
@@ -787,10 +788,10 @@
       <c r="B3" s="6"/>
       <c r="C3" s="14"/>
       <c r="D3" s="14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="12"/>
@@ -806,7 +807,7 @@
         <v>29</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="12"/>
@@ -819,10 +820,10 @@
       <c r="B5" s="8"/>
       <c r="C5" s="5"/>
       <c r="D5" s="14" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="N5" s="5"/>
     </row>
@@ -833,10 +834,10 @@
       <c r="B6" s="8"/>
       <c r="C6" s="5"/>
       <c r="D6" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N6" s="5"/>
     </row>
@@ -850,23 +851,23 @@
         <v>30</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="N7" s="5"/>
     </row>
-    <row r="8" spans="1:14" ht="238" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="255" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>43760</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="5"/>
       <c r="D8" s="14" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F8" s="10"/>
     </row>
@@ -876,7 +877,7 @@
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
notes for TPL added
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A296972F-E288-8A47-A6EE-2FA903463858}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57E3676-7506-A346-A22E-37A0209B785D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
   <si>
     <t>Algo</t>
   </si>
@@ -294,13 +294,6 @@
 CreditHours: 3.0;</t>
   </si>
   <si>
-    <t>Subject: Theory of Programming Languages;
-Instructor: Dr Amjad Mehmood;
-ClassSenior: +92 301 3068788‬;
-Note: Not prepared all lectures, but most of the syllabus comes from slides.;
-CreditHours: 3.0;</t>
-  </si>
-  <si>
     <t>Topic: name- Week 6,lectures- 1 Lecture, duration- 01:07;
 Video: link- https://drive.google.com/file/d/14EjJ9UzO_AGydV_w9UJIKyfJJMjCwjlW/preview, name- SRE Week#6, duration- 01:07;
 Slides: slide- Lecture Slide_4.pptx;
@@ -313,6 +306,46 @@
 Slides: slide- Lecture Slide_2.pptx;
 Topics: System and Context Boundaries, Context aspects in the system context, Defining System Boundary, Defining the Context Boundary, Documenting the System Context;
 Quiz: name- Quiz 1;</t>
+  </si>
+  <si>
+    <t>Subject: Theory of Programming Languages;
+Instructor: Dr Amjad Mehmood;
+ClassSenior: +92 301 3068788‬;
+Note: First 5 Chapters are included in Mid Term;
+CreditHours: 3.0;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 1, lectures- 3 Lectures, duration- 01:47;
+Video: link- https://drive.google.com/file/d/1ctSBf7a08q8Au16-1HEayw8aghDsauQG/preview, name- TPL Week#1 Part1, duration- 00:17;
+Video: link- https://drive.google.com/file/d/17yY-6RGVlhAsfMqJVqewvXUHGmNDlcR1/preview, name- TPL Week#1 Part2, duration- 00:53;
+Slides: slide- Chapter 1.ppt;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 2, lectures- 2 Lectures, duration- 01:40;
+Video: link- https://drive.google.com/file/d/15p5EP1_UCBHxyD9URakXw9xEW3hBKCLu/preview, name- TPL Week#2 Part 1, duration- 00:51;
+Video: link- https://drive.google.com/file/d/1hHFe7EcX_PNGHntkNqR0a4Q9tTmLY1d-/preview, name- TPL Week#2 Part 2, duration- 00:49;
+Important: 1 question will come from Chapter 2;
+Slides: slide- Chapter 2.ppt;
+Slides: slide- Chapter 3.ppt;
+Topics: Readability, reliability, writeability, Chapter 3, Lexemes, Backus Naur Form (BNF), Parse Trees;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 4, lectures- 1 Lecture, duration- 00:43;
+Video: link- https://drive.google.com/file/d/1JZjwQWO7_aTq04qMJLL5pf6HXNrv_qyN/preview, name- TPL Week#4, duration- 00:43;
+Slides: slide- Chapter 4.ppt;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 5, lectures- 1 Lecture, duration- 01:20;
+Video: link- https://drive.google.com/file/d/11P2oVuOQdNCB1lXC0azUnH74t3y6MwIx/preview, name- TPL Week#5, duration- 01:20;
+Slides: slide- Chapter 5.ppt</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 3, lectures- 1 Lecture, duration- 01:13;
+Video: link- https://drive.google.com/file/d/1Pu_2p-pfLQAGEPfub2GY7qYzCmXxi8LG/preview, name- TPL Week#3, duration- 01:13;
+Topics: EBNF, Attribute Grammer, EBNF Parse Trees;
+Important: Question can come that in words explain BNF,;
+Assignment: name- Assignment # 1 | Compare For Loops for Java with C++, img- /TPL/Assignment1.png;
+AssignmentSolution: name- Assignment 1 Solution | Compare For Loops, link- Assignment No 1 TPL Waqas 3151.docx;</t>
   </si>
 </sst>
 </file>
@@ -729,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB8366-CFB7-BD41-BAF1-2BC53FC93C19}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -769,7 +802,7 @@
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>33</v>
@@ -781,12 +814,14 @@
       <c r="G2" s="12"/>
       <c r="N2" s="6"/>
     </row>
-    <row r="3" spans="1:14" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>43720</v>
       </c>
       <c r="B3" s="6"/>
-      <c r="C3" s="14"/>
+      <c r="C3" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="D3" s="14" t="s">
         <v>32</v>
       </c>
@@ -797,12 +832,14 @@
       <c r="G3" s="12"/>
       <c r="N3" s="6"/>
     </row>
-    <row r="4" spans="1:14" ht="238" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="272" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
         <v>43724</v>
       </c>
       <c r="B4" s="6"/>
-      <c r="C4" s="14"/>
+      <c r="C4" s="14" t="s">
+        <v>46</v>
+      </c>
       <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
@@ -813,14 +850,16 @@
       <c r="G4" s="12"/>
       <c r="N4" s="6"/>
     </row>
-    <row r="5" spans="1:14" ht="238" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="272" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>43731</v>
       </c>
       <c r="B5" s="8"/>
-      <c r="C5" s="5"/>
+      <c r="C5" s="14" t="s">
+        <v>49</v>
+      </c>
       <c r="D5" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>34</v>
@@ -832,7 +871,9 @@
         <v>43739</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="5"/>
+      <c r="C6" s="14" t="s">
+        <v>47</v>
+      </c>
       <c r="D6" s="14" t="s">
         <v>31</v>
       </c>
@@ -846,7 +887,9 @@
         <v>43753</v>
       </c>
       <c r="B7" s="8"/>
-      <c r="C7" s="5"/>
+      <c r="C7" s="14" t="s">
+        <v>48</v>
+      </c>
       <c r="D7" s="14" t="s">
         <v>30</v>
       </c>
@@ -864,7 +907,7 @@
       <c r="B8" s="8"/>
       <c r="C8" s="5"/>
       <c r="D8" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E8" s="14" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
chapters 5 for TPL
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C673BF98-2569-EC43-BD41-4E7BC4789803}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3877C9F-F9D9-F643-8066-17FBC80E625E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
@@ -308,6 +308,13 @@
 Quiz: name- Quiz 1;</t>
   </si>
   <si>
+    <t>Subject: Theory of Programming Languages;
+Instructor: Dr Amjad Mehmood;
+ClassSenior: +92 301 3068788‬;
+Note: First 5 Chapters are included in Mid Term;
+CreditHours: 3.0;</t>
+  </si>
+  <si>
     <t>Topic: name- Week 4, lectures- 1 Lecture, duration- 00:43;
 Video: link- https://drive.google.com/file/d/1JZjwQWO7_aTq04qMJLL5pf6HXNrv_qyN/preview, name- TPL Week#4, duration- 00:43;
 Slides: slide- Chapter 4.ppt;</t>
@@ -340,13 +347,6 @@
 Video: link- https://drive.google.com/file/d/17yY-6RGVlhAsfMqJVqewvXUHGmNDlcR1/preview, name- TPL Week#1 Part2, duration- 00:53;
 Slides: slide- Chapter 1.ppt;
 Books: name- Concepts of Programming Languages 11th Ed.pdf, link- Concepts of Programming Languages 11th Ed.pdf</t>
-  </si>
-  <si>
-    <t>Subject: Theory of Programming Languages;
-Instructor: Dr Amjad Mehmood;
-ClassSenior: +92 301 3068788‬;
-Note: First 4 Chapters are included in Mid Term;
-CreditHours: 3.0;</t>
   </si>
 </sst>
 </file>
@@ -803,7 +803,7 @@
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="14" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>33</v>
@@ -821,7 +821,7 @@
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>32</v>
@@ -839,7 +839,7 @@
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>29</v>
@@ -857,7 +857,7 @@
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>43</v>
@@ -873,7 +873,7 @@
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>31</v>
@@ -889,7 +889,7 @@
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
fixed check for value exists
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3877C9F-F9D9-F643-8066-17FBC80E625E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12DED037-4A8C-C140-BC00-AC817AB33EA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
@@ -315,11 +315,6 @@
 CreditHours: 3.0;</t>
   </si>
   <si>
-    <t>Topic: name- Week 4, lectures- 1 Lecture, duration- 00:43;
-Video: link- https://drive.google.com/file/d/1JZjwQWO7_aTq04qMJLL5pf6HXNrv_qyN/preview, name- TPL Week#4, duration- 00:43;
-Slides: slide- Chapter 4.ppt;</t>
-  </si>
-  <si>
     <t>Topic: name- Week 5, lectures- 1 Lecture, duration- 01:20;
 Video: link- https://drive.google.com/file/d/11P2oVuOQdNCB1lXC0azUnH74t3y6MwIx/preview, name- TPL Week#5, duration- 01:20;
 Slides: slide- Chapter 5.ppt</t>
@@ -347,6 +342,10 @@
 Video: link- https://drive.google.com/file/d/17yY-6RGVlhAsfMqJVqewvXUHGmNDlcR1/preview, name- TPL Week#1 Part2, duration- 00:53;
 Slides: slide- Chapter 1.ppt;
 Books: name- Concepts of Programming Languages 11th Ed.pdf, link- Concepts of Programming Languages 11th Ed.pdf</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 4, lectures- 1 Lecture, duration- 00:43;
+Video: link- https://drive.google.com/file/d/1JZjwQWO7_aTq04qMJLL5pf6HXNrv_qyN/preview, name- TPL Week#4, duration- 00:43;</t>
   </si>
 </sst>
 </file>
@@ -763,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB8366-CFB7-BD41-BAF1-2BC53FC93C19}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -821,7 +820,7 @@
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>32</v>
@@ -839,7 +838,7 @@
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>29</v>
@@ -857,7 +856,7 @@
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>43</v>
@@ -873,7 +872,7 @@
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="14" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>31</v>
@@ -889,7 +888,7 @@
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>30</v>
@@ -919,7 +918,7 @@
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="D9" s="14"/>
       <c r="E9" s="14" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
added mid term course on web
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/QasimAli/nodejs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12DED037-4A8C-C140-BC00-AC817AB33EA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42CCDC13-C1D7-4442-86DC-EF9557C90560}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="23760" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="53">
   <si>
     <t>Algo</t>
   </si>
@@ -256,21 +256,6 @@
 Topics: String Searching domains, Valid and Invalid shifts, Symbols, Categories of Algorithums, a. Naive algorthims, b. Finite Automata;</t>
   </si>
   <si>
-    <t>Topic: name- Week 5,lectures- 2 Lectures, duration- 01:16;
-Video: link- https://drive.google.com/file/d/1t6VMFiI4610ULxoovPeFNuAnRKYwKosu/preview, name- AD&amp;AA Week#5 Part 1.mp4, duration- 00:25;
-Video: link- https://drive.google.com/file/d/1s_RbEVFMh9pGqPTkgfURH9Kx8nGcK3GI/preview, name- AD&amp;AA Week#5 Part 2.mp4, duration- 00:51;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 6,lectures- 2 Lectures, duration- 01:42;
-Video: link- https://drive.google.com/file/d/1rxg0O9yrSbrJpaYiql0F-P8u4Y2ZtDuc/preview, name- AD&amp;AA Week#6 Part 1.mp4, duration- 00:38;
-Video: link- https://drive.google.com/file/d/13r2bglsKWo9HeYgPDRZidU9CV5oJW6xu/preview, name- AD&amp;AA Week#6 Part 2.mp4, duration- 01:04;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 7,lectures- 2 Lectures, duration- 01:41;
-Video: link- https://drive.google.com/file/d/1iN0XDjE-kn0od8h8e3azwQFUaFEwDKEt/preview, name- AD&amp;AA Week#7 Part 1.mp4, duration- 00:57;
-Video: link- https://drive.google.com/file/d/130Cyy5mWSzIPNuH8qWlAk8wQcO5H_7o4/preview, name- AD&amp;AA Week#7 Part 2.mp4, duration- 00:44;</t>
-  </si>
-  <si>
     <t>Topic: name- Week 4,lectures- 1 Lecture, duration- 01:47;
 Video: link- https://drive.google.com/file/d/1lJBsIih3fzVFuQwubN4GLbkVKXgosBry/preview, name- AD&amp;AA Week#4.mp4, duration- 01:47;
 Topics: Knuth Morris Algorithum, Boyer Moore Algorithum, Algorithum time comparison;</t>
@@ -346,6 +331,47 @@
   <si>
     <t>Topic: name- Week 4, lectures- 1 Lecture, duration- 00:43;
 Video: link- https://drive.google.com/file/d/1JZjwQWO7_aTq04qMJLL5pf6HXNrv_qyN/preview, name- TPL Week#4, duration- 00:43;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 6,lectures- 2 Lectures, duration- 01:42;
+Video: link- https://drive.google.com/file/d/1rxg0O9yrSbrJpaYiql0F-P8u4Y2ZtDuc/preview, name- AD&amp;AA Week#6 Part 1.mp4, duration- 00:38;
+Video: link- https://drive.google.com/file/d/13r2bglsKWo9HeYgPDRZidU9CV5oJW6xu/preview, name- AD&amp;AA Week#6 Part 2.mp4, duration- 01:04;
+Slides: slide- lec3b.pptx;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 7,lectures- 2 Lectures, duration- 01:41;
+Video: link- https://drive.google.com/file/d/1iN0XDjE-kn0od8h8e3azwQFUaFEwDKEt/preview, name- AD&amp;AA Week#7 Part 1.mp4, duration- 00:57;
+Video: link- https://drive.google.com/file/d/130Cyy5mWSzIPNuH8qWlAk8wQcO5H_7o4/preview, name- AD&amp;AA Week#7 Part 2.mp4, duration- 00:44;
+Slides: slide- lec4.pptx;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 5,lectures- 2 Lectures, duration- 01:16;
+Video: link- https://drive.google.com/file/d/1t6VMFiI4610ULxoovPeFNuAnRKYwKosu/preview, name- AD&amp;AA Week#5 Part 1.mp4, duration- 00:25;
+Video: link- https://drive.google.com/file/d/1s_RbEVFMh9pGqPTkgfURH9Kx8nGcK3GI/preview, name- AD&amp;AA Week#5 Part 2.mp4, duration- 00:51;
+Slides: slide- lec3a.ppt</t>
+  </si>
+  <si>
+    <t>Topic: name- Mid Term Exam, lectures- , duration- 8 Nov | 16:00-17:30;
+Assignment: name- Mid Term Exam Pattern, img- /ALGO/paperpattern.png;
+Slides: slide- lec1.pptx;
+Slides: slide- lec2.pdf;
+Slides: slide- lec3b.pptx;</t>
+  </si>
+  <si>
+    <t>Topic: name- Mid Term Exam, lectures- , duration- 11 Nov | 15:00-16:30;
+Slides: slide- Chapter 1.ppt;
+Slides: slide- Chapter 2.ppt;
+Slides: slide- Chapter 3.ppt;
+Slides: slide- Chapter 5.pptx;
+Books: name- Concepts of Programming Languages 11th Ed, link- Concepts of Programming Languages 11th Ed.pdf;</t>
+  </si>
+  <si>
+    <t>Topic: name- Mid Term Exam, lectures- , duration- 12 Nov | 15:00-16:30;
+Slides: slide- Lecture Slide_1.pptx;
+Slides: slide- Lecture Slide_2.pptx;
+Slides: slide- Lecture Slide_3.pptx;
+Slides: slide- Lecture Slide_4.pptx;
+Books: name- Requirements Engineering Fundamentals, link- Requirements Engineering Fundamentals A Study Guide for the Certified Professional for Requirements Engineering Exam.pdf;</t>
   </si>
 </sst>
 </file>
@@ -762,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB8366-CFB7-BD41-BAF1-2BC53FC93C19}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -802,13 +828,13 @@
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>33</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="12"/>
@@ -820,13 +846,13 @@
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>32</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="12"/>
@@ -838,7 +864,7 @@
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>29</v>
@@ -856,10 +882,10 @@
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="14" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>34</v>
@@ -872,13 +898,13 @@
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>31</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="N6" s="5"/>
     </row>
@@ -888,13 +914,13 @@
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
@@ -905,30 +931,36 @@
         <v>43760</v>
       </c>
       <c r="B8" s="8"/>
-      <c r="C8" s="5"/>
+      <c r="C8" s="14" t="s">
+        <v>51</v>
+      </c>
       <c r="D8" s="14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="F8" s="10"/>
     </row>
-    <row r="9" spans="1:14" ht="153" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="170" x14ac:dyDescent="0.2">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="14"/>
+      <c r="D9" s="14" t="s">
+        <v>52</v>
+      </c>
       <c r="E9" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="119" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="E10" s="14" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="8"/>

</xml_diff>

<commit_message>
img position fixed. past paper added
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/QasimAli/nodejs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42CCDC13-C1D7-4442-86DC-EF9557C90560}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD363FC7-EEC9-D74B-81FB-C6D367A9B6FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="23760" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
@@ -367,6 +367,7 @@
   </si>
   <si>
     <t>Topic: name- Mid Term Exam, lectures- , duration- 12 Nov | 15:00-16:30;
+Assignment: name- Past Paper 2018, img- /SRE/mid exam past paper.jpeg;
 Slides: slide- Lecture Slide_1.pptx;
 Slides: slide- Lecture Slide_2.pptx;
 Slides: slide- Lecture Slide_3.pptx;
@@ -789,7 +790,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -840,7 +841,7 @@
       <c r="G2" s="12"/>
       <c r="N2" s="6"/>
     </row>
-    <row r="3" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>43720</v>
       </c>
@@ -942,7 +943,7 @@
       </c>
       <c r="F8" s="10"/>
     </row>
-    <row r="9" spans="1:14" ht="170" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="187" x14ac:dyDescent="0.2">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="5"/>

</xml_diff>

<commit_message>
mid paper date fixed
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/QasimAli/nodejs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD363FC7-EEC9-D74B-81FB-C6D367A9B6FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E35C74-EC02-864F-8FF5-FA5A385D4E00}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="23760" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
@@ -367,7 +367,7 @@
   </si>
   <si>
     <t>Topic: name- Mid Term Exam, lectures- , duration- 12 Nov | 15:00-16:30;
-Assignment: name- Past Paper 2018, img- /SRE/mid exam past paper.jpeg;
+Assignment: name- Past Paper 2017, img- /SRE/mid exam past paper.jpeg;
 Slides: slide- Lecture Slide_1.pptx;
 Slides: slide- Lecture Slide_2.pptx;
 Slides: slide- Lecture Slide_3.pptx;

</xml_diff>

<commit_message>
collapsed default functionality added
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/QasimAli/nodejs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E35C74-EC02-864F-8FF5-FA5A385D4E00}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A7A4BB-6E63-D442-BC39-441B5B98DE29}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="23760" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="54">
   <si>
     <t>Algo</t>
   </si>
@@ -373,6 +373,12 @@
 Slides: slide- Lecture Slide_3.pptx;
 Slides: slide- Lecture Slide_4.pptx;
 Books: name- Requirements Engineering Fundamentals, link- Requirements Engineering Fundamentals A Study Guide for the Certified Professional for Requirements Engineering Exam.pdf;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 6, lectures- 2 Lectures, duration- 01:42;
+Video: link- https://drive.google.com/file/d/1DJtOj-fOGE1gRrjlmTR0z7pvGFs5G7xU/preview, name- Part 1 Chapter 5 remaining, duration- 01:05;
+Video: link- https://drive.google.com/file/d/1aMmr-E7CAkgN8YMMwR4RX22u7qjPq6EH/preview, name- Part 2 Chapter 6 started, duration- 00:37;
+Topics: Variable life time, Variable scope, Chapter 6 Introduction;</t>
   </si>
 </sst>
 </file>
@@ -790,7 +796,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -933,7 +939,7 @@
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="14" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>39</v>
@@ -944,9 +950,13 @@
       <c r="F8" s="10"/>
     </row>
     <row r="9" spans="1:14" ht="187" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
+      <c r="A9" s="8">
+        <v>43775</v>
+      </c>
       <c r="B9" s="8"/>
-      <c r="C9" s="5"/>
+      <c r="C9" s="14" t="s">
+        <v>51</v>
+      </c>
       <c r="D9" s="14" t="s">
         <v>52</v>
       </c>

</xml_diff>

<commit_message>
added quiz for 2018
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/QasimAli/nodejs/renovationUpdates/server/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A7A4BB-6E63-D442-BC39-441B5B98DE29}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6CD1440-FFC3-9049-820F-7813B3670E26}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="23760" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -351,13 +351,6 @@
 Slides: slide- lec3a.ppt</t>
   </si>
   <si>
-    <t>Topic: name- Mid Term Exam, lectures- , duration- 8 Nov | 16:00-17:30;
-Assignment: name- Mid Term Exam Pattern, img- /ALGO/paperpattern.png;
-Slides: slide- lec1.pptx;
-Slides: slide- lec2.pdf;
-Slides: slide- lec3b.pptx;</t>
-  </si>
-  <si>
     <t>Topic: name- Mid Term Exam, lectures- , duration- 11 Nov | 15:00-16:30;
 Slides: slide- Chapter 1.ppt;
 Slides: slide- Chapter 2.ppt;
@@ -379,6 +372,14 @@
 Video: link- https://drive.google.com/file/d/1DJtOj-fOGE1gRrjlmTR0z7pvGFs5G7xU/preview, name- Part 1 Chapter 5 remaining, duration- 01:05;
 Video: link- https://drive.google.com/file/d/1aMmr-E7CAkgN8YMMwR4RX22u7qjPq6EH/preview, name- Part 2 Chapter 6 started, duration- 00:37;
 Topics: Variable life time, Variable scope, Chapter 6 Introduction;</t>
+  </si>
+  <si>
+    <t>Topic: name- Mid Term Exam, lectures- , duration- 8 Nov | 16:00-17:30;
+Assignment: name- Mid Term Exam Pattern, img- /ALGO/paperpattern.png;
+Assignment: name- Quiz photo from 2018, img- /ALGO/quiz2018.jpg;
+Slides: slide- lec1.pptx;
+Slides: slide- lec2.pdf;
+Slides: slide- lec3b.pptx;</t>
   </si>
 </sst>
 </file>
@@ -939,7 +940,7 @@
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>39</v>
@@ -955,22 +956,22 @@
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>51</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>52</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="119" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="153" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="14" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added solution and past paper
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6CD1440-FFC3-9049-820F-7813B3670E26}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{371918E0-047D-B443-A076-9B3336E3345A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -376,7 +376,10 @@
   <si>
     <t>Topic: name- Mid Term Exam, lectures- , duration- 8 Nov | 16:00-17:30;
 Assignment: name- Mid Term Exam Pattern, img- /ALGO/paperpattern.png;
-Assignment: name- Quiz photo from 2018, img- /ALGO/quiz2018.jpg;
+Assignment: name- Past Paper Mid Term (2018), img- /ALGO/quiz2018.jpg;
+Assignment: name- Solution 1 Question 1, img- /ALGO/mid2018soln1.png;
+Assignment: name- Solution 2 Question 1, img- /ALGO/mid2018soln1b.jpg;
+Assignment: name- Solution Question 2, img- /ALGO/mid2018soln2.png;
 Slides: slide- lec1.pptx;
 Slides: slide- lec2.pdf;
 Slides: slide- lec3b.pptx;</t>
@@ -796,7 +799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB8366-CFB7-BD41-BAF1-2BC53FC93C19}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -965,7 +968,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="153" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="255" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="5"/>

</xml_diff>

<commit_message>
saving changes with iteration function pending
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{371918E0-047D-B443-A076-9B3336E3345A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABB69F1-2D1F-EF42-A5F7-48C554B86DE6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -377,9 +377,7 @@
     <t>Topic: name- Mid Term Exam, lectures- , duration- 8 Nov | 16:00-17:30;
 Assignment: name- Mid Term Exam Pattern, img- /ALGO/paperpattern.png;
 Assignment: name- Past Paper Mid Term (2018), img- /ALGO/quiz2018.jpg;
-Assignment: name- Solution 1 Question 1, img- /ALGO/mid2018soln1.png;
-Assignment: name- Solution 2 Question 1, img- /ALGO/mid2018soln1b.jpg;
-Assignment: name- Solution Question 2, img- /ALGO/mid2018soln2.png;
+Assignment: name- Solution of Past Paper, img- /ALGO/mid2018soln1.png*/ALGO/mid2018soln1b.jpg*/ALGO/mid2018soln2.png*/ALGO/mid2018soln3a.jpg*/ALGO/mid2018soln3b.jpg*/ALGO/mid2018soln3c.jpg;
 Slides: slide- lec1.pptx;
 Slides: slide- lec2.pdf;
 Slides: slide- lec3b.pptx;</t>
@@ -968,7 +966,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="255" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="221" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="5"/>

</xml_diff>

<commit_message>
added past papers for tpl
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABB69F1-2D1F-EF42-A5F7-48C554B86DE6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE1D7B0-C912-F845-81CF-9C8F5A8D7974}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -351,14 +351,6 @@
 Slides: slide- lec3a.ppt</t>
   </si>
   <si>
-    <t>Topic: name- Mid Term Exam, lectures- , duration- 11 Nov | 15:00-16:30;
-Slides: slide- Chapter 1.ppt;
-Slides: slide- Chapter 2.ppt;
-Slides: slide- Chapter 3.ppt;
-Slides: slide- Chapter 5.pptx;
-Books: name- Concepts of Programming Languages 11th Ed, link- Concepts of Programming Languages 11th Ed.pdf;</t>
-  </si>
-  <si>
     <t>Topic: name- Mid Term Exam, lectures- , duration- 12 Nov | 15:00-16:30;
 Assignment: name- Past Paper 2017, img- /SRE/mid exam past paper.jpeg;
 Slides: slide- Lecture Slide_1.pptx;
@@ -381,6 +373,15 @@
 Slides: slide- lec1.pptx;
 Slides: slide- lec2.pdf;
 Slides: slide- lec3b.pptx;</t>
+  </si>
+  <si>
+    <t>Topic: name- Mid Term Exam, lectures- , duration- 11 Nov | 15:00-16:30;
+Assignment: name- Past paper 2018, img- /TPL/pastpaper1.jpg*/TPL/pastpaper2.jpg;
+Slides: slide- Chapter 1.ppt;
+Slides: slide- Chapter 2.ppt;
+Slides: slide- Chapter 3.ppt;
+Slides: slide- Chapter 5.pptx;
+Books: name- Concepts of Programming Languages 11th Ed, link- Concepts of Programming Languages 11th Ed.pdf;</t>
   </si>
 </sst>
 </file>
@@ -798,7 +799,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -941,7 +942,7 @@
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>39</v>
@@ -957,10 +958,10 @@
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>50</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>51</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>48</v>
@@ -972,7 +973,7 @@
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
chapters updated with videos
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8ADE8C-F102-F641-8021-B358EBBD5ECE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C965FF30-63C0-1840-B9D0-253EBEAB8311}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
@@ -300,37 +300,12 @@
 CreditHours: 3.0;</t>
   </si>
   <si>
-    <t>Topic: name- Week 5, lectures- 1 Lecture, duration- 01:20;
-Video: link- https://drive.google.com/file/d/11P2oVuOQdNCB1lXC0azUnH74t3y6MwIx/preview, name- TPL Week#5, duration- 01:20;
-Slides: slide- Chapter 5.ppt</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 2, lectures- 2 Lectures, duration- 01:40;
-Video: link- https://drive.google.com/file/d/15p5EP1_UCBHxyD9URakXw9xEW3hBKCLu/preview, name- TPL Week#2 Part 1, duration- 00:51;
-Video: link- https://drive.google.com/file/d/1hHFe7EcX_PNGHntkNqR0a4Q9tTmLY1d-/preview, name- TPL Week#2 Part 2, duration- 00:49;
-Slides: slide- Chapter 2.ppt;
-Slides: slide- Chapter 3.ppt;
-Topics: Readability, reliability, writeability, Chapter 3, Lexemes, Backus Naur Form (BNF), Parse Trees;
-Important: 1 question will come from Chapter 2;</t>
-  </si>
-  <si>
     <t>Topic: name- Week 3, lectures- 1 Lecture, duration- 01:13;
 Video: link- https://drive.google.com/file/d/1Pu_2p-pfLQAGEPfub2GY7qYzCmXxi8LG/preview, name- TPL Week#3, duration- 01:13;
 Assignment: name- Assignment # 1 | Compare For Loops for Java with C++, img- /TPL/Assignment1.png;
 AssignmentSolution: name- Assignment 1 Solution | Compare For Loops, link- Assignment No 1 TPL Waqas 3151.docx;
 Topics: EBNF, Attribute Grammer, EBNF Parse Trees;
 Important: Question can come "Explain BNF in words";</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 1, lectures- 3 Lectures, duration- 01:47;
-Video: link- https://drive.google.com/file/d/1ctSBf7a08q8Au16-1HEayw8aghDsauQG/preview, name- TPL Week#1 Part1, duration- 00:17;
-Video: link- https://drive.google.com/file/d/17yY-6RGVlhAsfMqJVqewvXUHGmNDlcR1/preview, name- TPL Week#1 Part2, duration- 00:53;
-Slides: slide- Chapter 1.ppt;
-Books: name- Concepts of Programming Languages 11th Ed.pdf, link- Concepts of Programming Languages 11th Ed.pdf</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 4, lectures- 1 Lecture, duration- 00:43;
-Video: link- https://drive.google.com/file/d/1JZjwQWO7_aTq04qMJLL5pf6HXNrv_qyN/preview, name- TPL Week#4, duration- 00:43;</t>
   </si>
   <si>
     <t>Topic: name- Week 6,lectures- 2 Lectures, duration- 01:42;
@@ -360,12 +335,6 @@
 Books: name- Requirements Engineering Fundamentals, link- Requirements Engineering Fundamentals A Study Guide for the Certified Professional for Requirements Engineering Exam.pdf;</t>
   </si>
   <si>
-    <t>Topic: name- Week 6, lectures- 2 Lectures, duration- 01:42;
-Video: link- https://drive.google.com/file/d/1DJtOj-fOGE1gRrjlmTR0z7pvGFs5G7xU/preview, name- Part 1 Chapter 5 remaining, duration- 01:05;
-Video: link- https://drive.google.com/file/d/1aMmr-E7CAkgN8YMMwR4RX22u7qjPq6EH/preview, name- Part 2 Chapter 6 started, duration- 00:37;
-Topics: Variable life time, Variable scope, Chapter 6 Introduction;</t>
-  </si>
-  <si>
     <t>Topic: name- Mid Term Exam, lectures- , duration- 8 Nov | 16:00-17:30;
 Assignment: name- Mid Term Exam Pattern, img- /ALGO/paperpattern.png;
 Assignment: name- Past Paper Mid Term (2018), img- /ALGO/quiz2018.jpg;
@@ -382,6 +351,40 @@
 Slides: slide- Chapter 3.ppt;
 Slides: slide- Chapter 5.pptx;
 Books: name- Concepts of Programming Languages 11th Ed, link- Concepts of Programming Languages 11th Ed.pdf;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 4, lectures- 1 Lecture, duration- 00:43;
+Video: link- https://drive.google.com/file/d/1JZjwQWO7_aTq04qMJLL5pf6HXNrv_qyN/preview, name- TPL Week#4, duration- 00:43;
+Topics: Compiler working flow chart, Top down parsing alogrithum, Construction of Syntaxtical Structure using BNF;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 6, lectures- 2 Lectures, duration- 01:42;
+Video: link- https://drive.google.com/file/d/1DJtOj-fOGE1gRrjlmTR0z7pvGFs5G7xU/preview, name- Part 1 Chapter 5 remaining, duration- 01:05;
+Video: link- https://drive.google.com/file/d/1aMmr-E7CAkgN8YMMwR4RX22u7qjPq6EH/preview, name- Part 2 Chapter 6 started, duration- 00:37;
+Topics: Variable life time, Variable scopes, Static Scope, Stack Dynamic scope, Explicit / implicit heap dynamic, Chapter 6 Introduction;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 1, lectures- 3 Lectures, duration- 01:47;
+Video: link- https://drive.google.com/file/d/1ctSBf7a08q8Au16-1HEayw8aghDsauQG/preview, name- TPL Week#1 Part1, duration- 00:17;
+Video: link- https://drive.google.com/file/d/17yY-6RGVlhAsfMqJVqewvXUHGmNDlcR1/preview, name- TPL Week#1 Part2, duration- 00:53;
+Slides: slide- Chapter 5.ppt;
+Books: name- Concepts of Programming Languages 11th Ed.pdf, link- Concepts of Programming Languages 11th Ed.pdf</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 2, lectures- 2 Lectures, duration- 01:40;
+Video: link- https://drive.google.com/file/d/15p5EP1_UCBHxyD9URakXw9xEW3hBKCLu/preview, name- TPL Week#2 Part 1, duration- 00:51;
+Video: link- https://drive.google.com/file/d/1hHFe7EcX_PNGHntkNqR0a4Q9tTmLY1d-/preview, name- TPL Week#2 Part 2, duration- 00:49;
+Slides: slide- Chapter 1.ppt;
+Slides: slide- Chapter 2.ppt;
+Slides: slide- Chapter 3.ppt;
+Topics: Readability, reliability, writeability, Chapter 3, Lexemes, Backus Naur Form (BNF), Parse Trees;
+Important: 1 question will come from Chapter 2;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 5, lectures- 1 Lecture, duration- 01:20;
+Video: link- https://drive.google.com/file/d/11P2oVuOQdNCB1lXC0azUnH74t3y6MwIx/preview, name- TPL Week#5, duration- 01:20;
+Slides: slide- Chapter 5.ppt;
+Topics: Context Free, Context Sensitive languages, Variable attributes, Possible binding times, Life time of a variable, Scope of a variable (example);</t>
   </si>
 </sst>
 </file>
@@ -798,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB8366-CFB7-BD41-BAF1-2BC53FC93C19}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -850,13 +853,13 @@
       <c r="G2" s="12"/>
       <c r="N2" s="6"/>
     </row>
-    <row r="3" spans="1:14" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>43720</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="14" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>32</v>
@@ -868,13 +871,13 @@
       <c r="G3" s="12"/>
       <c r="N3" s="6"/>
     </row>
-    <row r="4" spans="1:14" ht="272" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="289" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
         <v>43724</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="14" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>29</v>
@@ -892,7 +895,7 @@
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>40</v>
@@ -908,7 +911,7 @@
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="14" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>31</v>
@@ -924,13 +927,13 @@
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="14" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
@@ -942,13 +945,13 @@
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>39</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F8" s="10"/>
     </row>
@@ -958,13 +961,13 @@
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="14" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="221" x14ac:dyDescent="0.2">
@@ -973,7 +976,7 @@
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="14" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fixed img links mistake
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8127697-8502-1747-93A4-F269AB078FF1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F64977-6C82-6D44-B6F9-629FFF157828}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
@@ -385,7 +385,7 @@
 Slides: slide- Chapter 3.ppt;
 Slides: slide- Chapter 5.pptx;
 Books: name- Concepts of Programming Languages 11th Ed, link- Concepts of Programming Languages 11th Ed.pdf;
-Assignment: name- Mid Term Paper 2019, img- /TPL/mid20191.jpg*/TPL/mid20192.jpg*;</t>
+Assignment: name- Mid Term Paper 2019, img- /TPL/mid20191.jpg*/TPL/mid20192.jpg;</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
3 topics ch 3
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B44BF5-909C-914B-99F8-9B81FE9BC5FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5BB17B-CE3C-584D-85C0-7FAABB3C4563}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -386,7 +386,7 @@
 Slides: slide- Lecture Slide_3.pptx;
 Slides: slide- Lecture Slide_4.pptx;
 Books: name- Requirements Engineering Fundamentals, link- Requirements Engineering Fundamentals A Study Guide for the Certified Professional for Requirements Engineering Exam.pdf;
-Questions: Goals of requirements engineering, Core activities of requirements engineering, Characteristics of requirements engineer, Requirements types, Categorization of Quality Requirements, Aspects of system context, Documenting the system context</t>
+Questions: Goals of requirements engineering, Core activities of requirements engineering, Characteristics of requirements engineer, Requirements types, Categorization of Quality Requirements, Aspects of system context, Sources and Sinks of a system, Documenting the system context, Sources for elliciting requirements, Significance of stakeholders, Documenting stakeholders;</t>
   </si>
 </sst>
 </file>
@@ -804,7 +804,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -957,7 +957,7 @@
       </c>
       <c r="F8" s="10"/>
     </row>
-    <row r="9" spans="1:14" ht="272" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="306" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>43775</v>
       </c>

</xml_diff>

<commit_message>
2 topics ch 3 added
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF7D672-6AF3-8244-BF5A-8F885B9C3D61}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B25FE5-6460-F041-B31C-D07E1210C45B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
@@ -386,7 +386,7 @@
 Slides: slide- Lecture Slide_3.pptx;
 Slides: slide- Lecture Slide_4.pptx;
 Books: name- Requirements Engineering Fundamentals, link- Requirements Engineering Fundamentals A Study Guide for the Certified Professional for Requirements Engineering Exam.pdf;
-Questions: Goals of requirements engineering, Core activities of requirements engineering, Characteristics of requirements engineer, Requirements types, Categorization of Quality Requirements, Aspects of system context, Sources and Sinks of a system, Documenting the system context, Sources for elliciting requirements, Significance of stakeholders, Documenting stakeholders, Obligations of Requirements engineer, Previliges of stakeholders, Kano Model (Influence on requirements);</t>
+Questions: Goals of requirements engineering, Core activities of requirements engineering, Characteristics of requirements engineer, Requirements types, Categorization of Quality Requirements, Aspects of system context, Sources and Sinks of a system, Documenting the system context, Sources for elliciting requirements, Significance of stakeholders, Documenting stakeholders, Obligations of Requirements engineer, Previliges of stakeholders, Kano Model (Influence of requirements on sattisfaction), What influences selection of elicitation techniques;</t>
   </si>
 </sst>
 </file>
@@ -957,7 +957,7 @@
       </c>
       <c r="F8" s="10"/>
     </row>
-    <row r="9" spans="1:14" ht="340" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="356" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>43775</v>
       </c>

</xml_diff>

<commit_message>
added chapter 3 topics
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B25FE5-6460-F041-B31C-D07E1210C45B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BED443B-5978-334E-AC41-2F173406C15D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
@@ -386,7 +386,7 @@
 Slides: slide- Lecture Slide_3.pptx;
 Slides: slide- Lecture Slide_4.pptx;
 Books: name- Requirements Engineering Fundamentals, link- Requirements Engineering Fundamentals A Study Guide for the Certified Professional for Requirements Engineering Exam.pdf;
-Questions: Goals of requirements engineering, Core activities of requirements engineering, Characteristics of requirements engineer, Requirements types, Categorization of Quality Requirements, Aspects of system context, Sources and Sinks of a system, Documenting the system context, Sources for elliciting requirements, Significance of stakeholders, Documenting stakeholders, Obligations of Requirements engineer, Previliges of stakeholders, Kano Model (Influence of requirements on sattisfaction), What influences selection of elicitation techniques;</t>
+Questions: Goals of requirements engineering, Core activities of requirements engineering, Characteristics of requirements engineer, Requirements types, Categorization of Quality Requirements, Aspects of system context, Sources and Sinks of a system, Documenting the system context, Sources for elliciting requirements, Significance of stakeholders, Documenting stakeholders, Obligations of Requirements engineer, Previliges of stakeholders, Kano Model (Influence of requirements on sattisfaction), What influences selection of elicitation techniques, Human influences, Observation influence, Operational influence, Combining ellicitations techniques to lower risk, Interview, Questionaire, Creative techniques types, Brainstorming &amp; paradox, System archeology, Perspective based reading, Questions observation &amp; optimize process, Field observation, Apprenticing, Types of support techniques, Modelling action sequences;</t>
   </si>
 </sst>
 </file>
@@ -957,7 +957,7 @@
       </c>
       <c r="F8" s="10"/>
     </row>
-    <row r="9" spans="1:14" ht="356" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>43775</v>
       </c>

</xml_diff>

<commit_message>
separator for chapter added
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BED443B-5978-334E-AC41-2F173406C15D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B56D87D-74B6-DC48-B996-833BD73A8E59}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
@@ -386,7 +386,7 @@
 Slides: slide- Lecture Slide_3.pptx;
 Slides: slide- Lecture Slide_4.pptx;
 Books: name- Requirements Engineering Fundamentals, link- Requirements Engineering Fundamentals A Study Guide for the Certified Professional for Requirements Engineering Exam.pdf;
-Questions: Goals of requirements engineering, Core activities of requirements engineering, Characteristics of requirements engineer, Requirements types, Categorization of Quality Requirements, Aspects of system context, Sources and Sinks of a system, Documenting the system context, Sources for elliciting requirements, Significance of stakeholders, Documenting stakeholders, Obligations of Requirements engineer, Previliges of stakeholders, Kano Model (Influence of requirements on sattisfaction), What influences selection of elicitation techniques, Human influences, Observation influence, Operational influence, Combining ellicitations techniques to lower risk, Interview, Questionaire, Creative techniques types, Brainstorming &amp; paradox, System archeology, Perspective based reading, Questions observation &amp; optimize process, Field observation, Apprenticing, Types of support techniques, Modelling action sequences;</t>
+Questions: Chapter 1, Goals of requirements engineering, Core activities of requirements engineering, Characteristics of requirements engineer, Requirements types, Categorization of Quality Requirements, Chapter 2, Aspects of system context, Sources and Sinks of a system, Documenting the system context, Chapter 3, Sources for elliciting requirements, Significance of stakeholders, Documenting stakeholders, Obligations of Requirements engineer, Previliges of stakeholders, Kano Model (Influence of requirements on sattisfaction), What influences selection of elicitation techniques, Human influences, Observation influence, Operational influence, Combining ellicitations techniques to lower risk, Interview, Questionaire, Creative techniques types, Brainstorming &amp; paradox, System archeology, Perspective based reading, Questions observation &amp; optimize process, Field observation, Apprenticing, Types of support techniques, Modelling action sequences;</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
added chapter 4 contents
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B56D87D-74B6-DC48-B996-833BD73A8E59}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A002F0E6-E46F-9A4D-83FA-2452F803C5D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -386,7 +386,7 @@
 Slides: slide- Lecture Slide_3.pptx;
 Slides: slide- Lecture Slide_4.pptx;
 Books: name- Requirements Engineering Fundamentals, link- Requirements Engineering Fundamentals A Study Guide for the Certified Professional for Requirements Engineering Exam.pdf;
-Questions: Chapter 1, Goals of requirements engineering, Core activities of requirements engineering, Characteristics of requirements engineer, Requirements types, Categorization of Quality Requirements, Chapter 2, Aspects of system context, Sources and Sinks of a system, Documenting the system context, Chapter 3, Sources for elliciting requirements, Significance of stakeholders, Documenting stakeholders, Obligations of Requirements engineer, Previliges of stakeholders, Kano Model (Influence of requirements on sattisfaction), What influences selection of elicitation techniques, Human influences, Observation influence, Operational influence, Combining ellicitations techniques to lower risk, Interview, Questionaire, Creative techniques types, Brainstorming &amp; paradox, System archeology, Perspective based reading, Questions observation &amp; optimize process, Field observation, Apprenticing, Types of support techniques, Modelling action sequences;</t>
+Questions: Chapter 1, Goals of requirements engineering, Core activities of requirements engineering, Characteristics of requirements engineer, Requirements types, Categorization of Quality Requirements, Chapter 2, Aspects of system context, Sources and Sinks of a system, Documenting the system context, Chapter 3, Sources for elliciting requirements, Significance of stakeholders, Documenting stakeholders, Obligations of Requirements engineer, Previliges of stakeholders, Kano Model (Influence of requirements on sattisfaction), What influences selection of elicitation techniques, Human influences, Observation influence, Operational influence, Combining ellicitations techniques to lower risk, Interview, Questionaire, Creative techniques types, Brainstorming &amp; paradox, System archeology, Perspective based reading, Questions observation &amp; optimize process, Field observation, Apprenticing, Types of support techniques, Modelling action sequences, Chapter 4, Reason for documentations, Documentation Perspectives (Types), Advantages of using natural languages, 4 Conceptual Models, Standardized Structring Advantages, Names of different Standards (3), Parts of ISO 29148 Standard Document, Parts of Customized Standard Contents, Parts of introduction in custom standards, Parts of General Overview in Custom standards, Uses of requirements documents, Quality criteria for requirements documents;</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
week 7 updated on 15 Nov
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D05A04-115B-C94F-BF31-339030AE08BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46AC6509-168B-C744-9FF0-35C8DD59F753}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
   <si>
     <t>Algo</t>
   </si>
@@ -222,6 +222,178 @@
 Topics: Eliciting Requirements Sources, Documenting Stakeholders, Obligations of requirements Engineer, Obligations of stakeholders, Kano Model, Categories of satisfaction, Satisfiers, Delighters, Dissatisfiers, Elicitation Techniques (Introduction), Influencing factors regarding the choice of elicitation techniques;</t>
   </si>
   <si>
+    <t>Topic: name- Week 3,lectures- 3 Lectures, duration- 01:03;
+Video: link- https://drive.google.com/file/d/1kKy4hXIJKfQ2hLfVO1ScYWFaF0kz20Yv/preview, name- AD&amp;AA Week#3 Part1.mp4, duration- 00:35;
+Video: link- https://drive.google.com/file/d/1m6Ryy3hVXhK3BKsZmLCoqm6Vlql0ACJY/preview, name- AD&amp;AA Week#3 Part2.mp4, duration- 00:16;
+Video: link- https://drive.google.com/file/d/1-K9i4B1zTrsZYJozlIXuPo-NcThHbt3S/preview, name- AD&amp;AA Week#3 Part3.mp4, duration- 00:12;
+Topics: Finite Automata (continued);</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 2,lectures- 2 Lectures, duration- 01:36;
+Video: link- https://drive.google.com/file/d/1bRNxpWytwwu50SDsvaOXaxXAWO5r8-B8/preview, name- AD&amp;AA Week#2 Part1.mp4, duration- 01:05;
+Video: link- https://drive.google.com/file/d/1eiOj0evGS4VLvvaoCQFeEQzat_4W_uDq/preview, name- AD&amp;AA Week#2 Part2.mp4, duration- 00:31;
+Slides: slide- lec2.pdf;
+Topics: String Searching domains, Valid and Invalid shifts, Symbols, Categories of Algorithums, a. Naive algorthims, b. Finite Automata;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 4,lectures- 1 Lecture, duration- 01:47;
+Video: link- https://drive.google.com/file/d/1lJBsIih3fzVFuQwubN4GLbkVKXgosBry/preview, name- AD&amp;AA Week#4.mp4, duration- 01:47;
+Topics: Knuth Morris Algorithum, Boyer Moore Algorithum, Algorithum time comparison;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 1,lectures- 4 Lectures, duration- 01:38;
+Video: link- https://drive.google.com/file/d/1rba7mKiAH4UScARCW3HuCe5_LsdgofF_/preview, name- Class CR Number, duration- 00:00;
+Video: link- https://drive.google.com/file/d/1EvOHehNqZlji9HeyW6YYI6pGN-apUz8D/preview, name- AD&amp;AA Week#1 Part1.mp4, duration- 00:58;
+Video: link- https://drive.google.com/file/d/1PQ9EuYIsfZiHfxVupjg5JThWLEUT-1ka/preview, name- AD&amp;AA Week#1 Part2.mp4, duration- 00:32;
+Video: link- https://drive.google.com/file/d/1RfT5B3ulAR_QIrI8ktEg9r5u-FHZFxa3/preview, name- AD&amp;AA Week#1 Part3.mp4, duration- 00:14;
+Slides: slide- lec1.pptx;
+Assignment: name- Assignment # 1 Summary of Cincinati Website , link- /ALGO/cincinati.png;
+Assignment: name- Assignment # 2 Load Bty 18650 Algorithum , link- /ALGO/18650.png;
+Topics: Definition of Algorithum, Types of Algorithums, Flow Diagram Symbols, e la russ algorithum, Divide and COnquor algorithum, Parameters for selection of algorithum, e la russ algorithum if statements;</t>
+  </si>
+  <si>
+    <t>Subject: Advance Theory and Design of Algorithum;
+Instructor: Dr Aqib Perwaiz;
+ClassSenior: Jasim, +92 323 4154345;
+Note: Listening to all lectures is necessary. Sir teaches most of the stuff on slides.;
+CreditHours: 3.0;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 6,lectures- 1 Lecture, duration- 01:07;
+Video: link- https://drive.google.com/file/d/14EjJ9UzO_AGydV_w9UJIKyfJJMjCwjlW/preview, name- SRE Week#6, duration- 01:07;
+Slides: slide- Lecture Slide_4.pptx;
+Topics: Document Design, Reasons for documentation, a. Central role of requirements, b. Legal relevance, c. Complexity, d. Accessibility, Types of Documentation, a. Data perspective, b. Functional perspective, c. Behaviourial perspective, Advantages of using natural language, Disadvantages of using natural language,  Requirements Documentation using Conceptual Models, a. Use case diagram, b. Structural data modeling and structuring of terms class diagram, c. Sequence modelling, d. State diagram, Hybrid Requirements Documents;
+Quiz: name- Quiz 2;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 3,lectures- 1 Lecture, duration- 01:03;
+Video: link- https://drive.google.com/file/d/1f-_LejqI4_0bTJl9ld5vK7xt1ftYtFt5/preview, name- SRE Week#3, duration- 01:03;
+Slides: slide- Lecture Slide_2.pptx;
+Topics: System and Context Boundaries, Context aspects in the system context, Defining System Boundary, Defining the Context Boundary, Documenting the System Context;
+Quiz: name- Quiz 1;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 3, lectures- 1 Lecture, duration- 01:13;
+Video: link- https://drive.google.com/file/d/1Pu_2p-pfLQAGEPfub2GY7qYzCmXxi8LG/preview, name- TPL Week#3, duration- 01:13;
+Assignment: name- Assignment # 1 | Compare For Loops for Java with C++, img- /TPL/Assignment1.png;
+AssignmentSolution: name- Assignment 1 Solution | Compare For Loops, link- Assignment No 1 TPL Waqas 3151.docx;
+Topics: EBNF, Attribute Grammer, EBNF Parse Trees;
+Important: Question can come "Explain BNF in words";</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 6,lectures- 2 Lectures, duration- 01:42;
+Video: link- https://drive.google.com/file/d/1rxg0O9yrSbrJpaYiql0F-P8u4Y2ZtDuc/preview, name- AD&amp;AA Week#6 Part 1.mp4, duration- 00:38;
+Video: link- https://drive.google.com/file/d/13r2bglsKWo9HeYgPDRZidU9CV5oJW6xu/preview, name- AD&amp;AA Week#6 Part 2.mp4, duration- 01:04;
+Slides: slide- lec3b.pptx;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 7,lectures- 2 Lectures, duration- 01:41;
+Video: link- https://drive.google.com/file/d/1iN0XDjE-kn0od8h8e3azwQFUaFEwDKEt/preview, name- AD&amp;AA Week#7 Part 1.mp4, duration- 00:57;
+Video: link- https://drive.google.com/file/d/130Cyy5mWSzIPNuH8qWlAk8wQcO5H_7o4/preview, name- AD&amp;AA Week#7 Part 2.mp4, duration- 00:44;
+Slides: slide- lec4.pptx;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 5,lectures- 2 Lectures, duration- 01:16;
+Video: link- https://drive.google.com/file/d/1t6VMFiI4610ULxoovPeFNuAnRKYwKosu/preview, name- AD&amp;AA Week#5 Part 1.mp4, duration- 00:25;
+Video: link- https://drive.google.com/file/d/1s_RbEVFMh9pGqPTkgfURH9Kx8nGcK3GI/preview, name- AD&amp;AA Week#5 Part 2.mp4, duration- 00:51;
+Slides: slide- lec3a.ppt</t>
+  </si>
+  <si>
+    <t>Topic: name- Mid Term Exam, lectures- , duration- 8 Nov | 16:00-17:30;
+Assignment: name- Mid Term Exam Pattern, img- /ALGO/paperpattern.png;
+Assignment: name- Past Paper Mid Term (2018), img- /ALGO/quiz2018.jpg;
+Assignment: name- Solution of Past Paper, img- /ALGO/mid2018soln1.png*/ALGO/mid2018soln1b.jpg*/ALGO/mid2018soln2.png*/ALGO/mid2018soln3a.jpg*/ALGO/mid2018soln3b.jpg*/ALGO/mid2018soln3c.jpg;
+Slides: slide- lec1.pptx;
+Slides: slide- lec2.pdf;
+Slides: slide- lec3b.pptx;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 4, lectures- 1 Lecture, duration- 00:43;
+Video: link- https://drive.google.com/file/d/1JZjwQWO7_aTq04qMJLL5pf6HXNrv_qyN/preview, name- TPL Week#4, duration- 00:43;
+Topics: Compiler working flow chart, Top down parsing alogrithum, Construction of Syntaxtical Structure using BNF;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 6, lectures- 2 Lectures, duration- 01:42;
+Video: link- https://drive.google.com/file/d/1DJtOj-fOGE1gRrjlmTR0z7pvGFs5G7xU/preview, name- Part 1 Chapter 5 remaining, duration- 01:05;
+Video: link- https://drive.google.com/file/d/1aMmr-E7CAkgN8YMMwR4RX22u7qjPq6EH/preview, name- Part 2 Chapter 6 started, duration- 00:37;
+Topics: Variable life time, Variable scopes, Static Scope, Stack Dynamic scope, Explicit / implicit heap dynamic, Chapter 6 Introduction;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 1, lectures- 3 Lectures, duration- 01:47;
+Video: link- https://drive.google.com/file/d/1ctSBf7a08q8Au16-1HEayw8aghDsauQG/preview, name- TPL Week#1 Part1, duration- 00:17;
+Video: link- https://drive.google.com/file/d/17yY-6RGVlhAsfMqJVqewvXUHGmNDlcR1/preview, name- TPL Week#1 Part2, duration- 00:53;
+Slides: slide- Chapter 5.ppt;
+Books: name- Concepts of Programming Languages 11th Ed.pdf, link- Concepts of Programming Languages 11th Ed.pdf</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 2, lectures- 2 Lectures, duration- 01:40;
+Video: link- https://drive.google.com/file/d/15p5EP1_UCBHxyD9URakXw9xEW3hBKCLu/preview, name- TPL Week#2 Part 1, duration- 00:51;
+Video: link- https://drive.google.com/file/d/1hHFe7EcX_PNGHntkNqR0a4Q9tTmLY1d-/preview, name- TPL Week#2 Part 2, duration- 00:49;
+Slides: slide- Chapter 1.ppt;
+Slides: slide- Chapter 2.ppt;
+Slides: slide- Chapter 3.ppt;
+Topics: Readability, reliability, writeability, Chapter 3, Lexemes, Backus Naur Form (BNF), Parse Trees;
+Important: 1 question will come from Chapter 2;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 5, lectures- 1 Lecture, duration- 01:20;
+Video: link- https://drive.google.com/file/d/11P2oVuOQdNCB1lXC0azUnH74t3y6MwIx/preview, name- TPL Week#5, duration- 01:20;
+Slides: slide- Chapter 5.ppt;
+Topics: Context Free, Context Sensitive languages, Variable attributes, Possible binding times, Life time of a variable, Scope of a variable (example);</t>
+  </si>
+  <si>
+    <t>Topic: name- Mid Term Exam, lectures- , duration- 11 Nov | 15:00-16:30;
+Assignment: name- Past paper 2018, img- /TPL/pastpaper1.jpg*/TPL/pastpaper2.jpg;
+Slides: slide- Chapter 1.ppt;
+Slides: slide- Chapter 2.ppt;
+Slides: slide- Chapter 3.ppt;
+Slides: slide- Chapter 5.pptx;
+Books: name- Concepts of Programming Languages 11th Ed, link- Concepts of Programming Languages 11th Ed.pdf;
+Assignment: name- Mid Term Paper 2019, img- /TPL/mid20191.jpg*/TPL/mid20192.jpg;</t>
+  </si>
+  <si>
+    <t>Topic: name- Mid Term Exam, lectures- , duration- 12 Nov | 15:00-16:30;
+Assignment: name- Past Paper 2017, img- /SRE/mid exam past paper.jpeg;
+Slides: slide- Lecture Slide_1.pptx;
+Slides: slide- Lecture Slide_2.pptx;
+Slides: slide- Lecture Slide_3.pptx;
+Slides: slide- Lecture Slide_4.pptx;
+Books: name- Requirements Engineering Fundamentals, link- Requirements Engineering Fundamentals A Study Guide for the Certified Professional for Requirements Engineering Exam.pdf;
+Questions: Chapter 1, Goals of requirements engineering, Core activities of requirements engineering, Characteristics of requirements engineer, Requirements types, Categorization of Quality Requirements, Chapter 2, Aspects of system context, Sources and Sinks of a system, Documenting the system context, Chapter 3, Sources for elliciting requirements, Significance of stakeholders, Documenting stakeholders, Obligations of Requirements engineer, Previliges of stakeholders, Kano Model (Influence of requirements on sattisfaction), What influences selection of elicitation techniques, Human influences, Observation influence, Operational influence, Combining ellicitations techniques to lower risk, Interview, Questionaire, Creative techniques types, Brainstorming &amp; paradox, System archeology, Perspective based reading, Questions observation &amp; optimize process, Field observation, Apprenticing, Types of support techniques, Modelling action sequences, Chapter 4, Reason for documentations, Documentation Perspectives (Types), Advantages of using natural languages, 4 Conceptual Models, Standardized Structring Advantages, Names of different Standards (3), Parts of ISO 29148 Standard Document, Parts of Customized Standard Contents, Parts of introduction in custom standards, Parts of General Overview in Custom standards, Uses of requirements documents, Quality criteria for requirements documents;</t>
+  </si>
+  <si>
+    <t>IS</t>
+  </si>
+  <si>
+    <t>Subject: Special Topics in Information Security;
+Instructor: Dr Syed Nasir Mehmood Shah;
+ClassSenior: Waqas Wattoo | +92 301 3068788;
+Note: None yet;
+CreditHours: 3.0;</t>
+  </si>
+  <si>
+    <t>Topic: name- Course Material,lectures- 5 Lectures, duration- 00;
+Slides: slide- An Analysis of Security Threats in Cloud Computing.pptx;
+Slides: slide- Lecture1_Information Security.pdf;
+Slides: slide- Lecture2_SecureCloudFramework.pdf;
+Slides: slide- Lecture3_EmergingTrendsinCloudSecurity.pdf;
+Slides: slide- Muhammad Sadiq Thesis v1.7.pdf;</t>
+  </si>
+  <si>
+    <t>Subject: Theory of Programming Languages;
+Instructor: Dr Amjad Mehmood;
+ClassSenior: +92 301 3068788‬;
+Note: No lecture on 16 Nov due to papers;
+CreditHours: 3.0;</t>
+  </si>
+  <si>
+    <t>Subject: Software Requirement Engineering;
+Instructor: Mr Fazal Wahab;
+ClassSenior: Fakhar | +92 ‭332 0278998‬;
+Note: No lecture on 16 Nov due to papers;
+CreditHours: 3.0;</t>
+  </si>
+  <si>
     <t>Topic: name- Week 1,lectures- 3 Lectures, duration- 01:47;
 Video: link- https://drive.google.com/file/d/1brUQVmv6OGb2n1GePe4c5fjrVbVJUFvz/preview, name- Class CR Number, duration- 00:04;
 Video: link- https://drive.google.com/file/d/1-oeLFxAxdOeAgkILn1uyLbTcr-NsZlIT/preview, name- SRE Week#1 Part1.mp4, duration- 56:47;
@@ -231,180 +403,22 @@
 Books: name- Requirements Engineering Fundamentals A Study Guide for the Certified Professional for Requirements Engineering Exam, link- Requirements Engineering Fundamentals A Study Guide for the Certified Professional for Requirements Engineering Exam.pdf;
 Books: name- Requirements Engineering a good practice guide by Ian Sommervilla &amp; Pete Sawyer;
 Books: name- Software Requirements 3rd Edtion by Xarl Wuuigers &amp; Joy Beatty;
-Books: name- Engineering &amp; Managing Software Requirements by Ayubuke Aurum &amp; Class Wohlin; 
-Assignment: name- Assignment # 1 , link- Assignment No.1 2.pdf;</t>
-  </si>
-  <si>
-    <t>Subject: Software Requirement Engineering;
-Instructor: Mr Fazal Wahab;
-ClassSenior: Fakhar | +92 ‭332 0278998‬;
-Note: Most of the questions in papers will come from slides. If we prepare slides only we will make it.;
-CreditHours: 3.0;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 3,lectures- 3 Lectures, duration- 01:03;
-Video: link- https://drive.google.com/file/d/1kKy4hXIJKfQ2hLfVO1ScYWFaF0kz20Yv/preview, name- AD&amp;AA Week#3 Part1.mp4, duration- 00:35;
-Video: link- https://drive.google.com/file/d/1m6Ryy3hVXhK3BKsZmLCoqm6Vlql0ACJY/preview, name- AD&amp;AA Week#3 Part2.mp4, duration- 00:16;
-Video: link- https://drive.google.com/file/d/1-K9i4B1zTrsZYJozlIXuPo-NcThHbt3S/preview, name- AD&amp;AA Week#3 Part3.mp4, duration- 00:12;
-Topics: Finite Automata (continued);</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 2,lectures- 2 Lectures, duration- 01:36;
-Video: link- https://drive.google.com/file/d/1bRNxpWytwwu50SDsvaOXaxXAWO5r8-B8/preview, name- AD&amp;AA Week#2 Part1.mp4, duration- 01:05;
-Video: link- https://drive.google.com/file/d/1eiOj0evGS4VLvvaoCQFeEQzat_4W_uDq/preview, name- AD&amp;AA Week#2 Part2.mp4, duration- 00:31;
-Slides: slide- lec2.pdf;
-Topics: String Searching domains, Valid and Invalid shifts, Symbols, Categories of Algorithums, a. Naive algorthims, b. Finite Automata;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 4,lectures- 1 Lecture, duration- 01:47;
-Video: link- https://drive.google.com/file/d/1lJBsIih3fzVFuQwubN4GLbkVKXgosBry/preview, name- AD&amp;AA Week#4.mp4, duration- 01:47;
-Topics: Knuth Morris Algorithum, Boyer Moore Algorithum, Algorithum time comparison;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 1,lectures- 4 Lectures, duration- 01:38;
-Video: link- https://drive.google.com/file/d/1rba7mKiAH4UScARCW3HuCe5_LsdgofF_/preview, name- Class CR Number, duration- 00:00;
-Video: link- https://drive.google.com/file/d/1EvOHehNqZlji9HeyW6YYI6pGN-apUz8D/preview, name- AD&amp;AA Week#1 Part1.mp4, duration- 00:58;
-Video: link- https://drive.google.com/file/d/1PQ9EuYIsfZiHfxVupjg5JThWLEUT-1ka/preview, name- AD&amp;AA Week#1 Part2.mp4, duration- 00:32;
-Video: link- https://drive.google.com/file/d/1RfT5B3ulAR_QIrI8ktEg9r5u-FHZFxa3/preview, name- AD&amp;AA Week#1 Part3.mp4, duration- 00:14;
-Slides: slide- lec1.pptx;
-Assignment: name- Assignment # 1 Summary of Cincinati Website , link- /ALGO/cincinati.png;
-Assignment: name- Assignment # 2 Load Bty 18650 Algorithum , link- /ALGO/18650.png;
-Topics: Definition of Algorithum, Types of Algorithums, Flow Diagram Symbols, e la russ algorithum, Divide and COnquor algorithum, Parameters for selection of algorithum, e la russ algorithum if statements;</t>
-  </si>
-  <si>
-    <t>Subject: Advance Theory and Design of Algorithum;
-Instructor: Dr Aqib Perwaiz;
-ClassSenior: Jasim, +92 323 4154345;
-Note: Listening to all lectures is necessary. Sir teaches most of the stuff on slides.;
-CreditHours: 3.0;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 6,lectures- 1 Lecture, duration- 01:07;
-Video: link- https://drive.google.com/file/d/14EjJ9UzO_AGydV_w9UJIKyfJJMjCwjlW/preview, name- SRE Week#6, duration- 01:07;
-Slides: slide- Lecture Slide_4.pptx;
-Topics: Document Design, Reasons for documentation, a. Central role of requirements, b. Legal relevance, c. Complexity, d. Accessibility, Types of Documentation, a. Data perspective, b. Functional perspective, c. Behaviourial perspective, Advantages of using natural language, Disadvantages of using natural language,  Requirements Documentation using Conceptual Models, a. Use case diagram, b. Structural data modeling and structuring of terms class diagram, c. Sequence modelling, d. State diagram, Hybrid Requirements Documents;
-Quiz: name- Quiz 2;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 3,lectures- 1 Lecture, duration- 01:03;
-Video: link- https://drive.google.com/file/d/1f-_LejqI4_0bTJl9ld5vK7xt1ftYtFt5/preview, name- SRE Week#3, duration- 01:03;
-Slides: slide- Lecture Slide_2.pptx;
-Topics: System and Context Boundaries, Context aspects in the system context, Defining System Boundary, Defining the Context Boundary, Documenting the System Context;
-Quiz: name- Quiz 1;</t>
-  </si>
-  <si>
-    <t>Subject: Theory of Programming Languages;
-Instructor: Dr Amjad Mehmood;
-ClassSenior: +92 301 3068788‬;
-Note: First 5 Chapters are included in Mid Term;
-CreditHours: 3.0;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 3, lectures- 1 Lecture, duration- 01:13;
-Video: link- https://drive.google.com/file/d/1Pu_2p-pfLQAGEPfub2GY7qYzCmXxi8LG/preview, name- TPL Week#3, duration- 01:13;
-Assignment: name- Assignment # 1 | Compare For Loops for Java with C++, img- /TPL/Assignment1.png;
-AssignmentSolution: name- Assignment 1 Solution | Compare For Loops, link- Assignment No 1 TPL Waqas 3151.docx;
-Topics: EBNF, Attribute Grammer, EBNF Parse Trees;
-Important: Question can come "Explain BNF in words";</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 6,lectures- 2 Lectures, duration- 01:42;
-Video: link- https://drive.google.com/file/d/1rxg0O9yrSbrJpaYiql0F-P8u4Y2ZtDuc/preview, name- AD&amp;AA Week#6 Part 1.mp4, duration- 00:38;
-Video: link- https://drive.google.com/file/d/13r2bglsKWo9HeYgPDRZidU9CV5oJW6xu/preview, name- AD&amp;AA Week#6 Part 2.mp4, duration- 01:04;
-Slides: slide- lec3b.pptx;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 7,lectures- 2 Lectures, duration- 01:41;
-Video: link- https://drive.google.com/file/d/1iN0XDjE-kn0od8h8e3azwQFUaFEwDKEt/preview, name- AD&amp;AA Week#7 Part 1.mp4, duration- 00:57;
-Video: link- https://drive.google.com/file/d/130Cyy5mWSzIPNuH8qWlAk8wQcO5H_7o4/preview, name- AD&amp;AA Week#7 Part 2.mp4, duration- 00:44;
-Slides: slide- lec4.pptx;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 5,lectures- 2 Lectures, duration- 01:16;
-Video: link- https://drive.google.com/file/d/1t6VMFiI4610ULxoovPeFNuAnRKYwKosu/preview, name- AD&amp;AA Week#5 Part 1.mp4, duration- 00:25;
-Video: link- https://drive.google.com/file/d/1s_RbEVFMh9pGqPTkgfURH9Kx8nGcK3GI/preview, name- AD&amp;AA Week#5 Part 2.mp4, duration- 00:51;
-Slides: slide- lec3a.ppt</t>
-  </si>
-  <si>
-    <t>Topic: name- Mid Term Exam, lectures- , duration- 8 Nov | 16:00-17:30;
-Assignment: name- Mid Term Exam Pattern, img- /ALGO/paperpattern.png;
-Assignment: name- Past Paper Mid Term (2018), img- /ALGO/quiz2018.jpg;
-Assignment: name- Solution of Past Paper, img- /ALGO/mid2018soln1.png*/ALGO/mid2018soln1b.jpg*/ALGO/mid2018soln2.png*/ALGO/mid2018soln3a.jpg*/ALGO/mid2018soln3b.jpg*/ALGO/mid2018soln3c.jpg;
-Slides: slide- lec1.pptx;
-Slides: slide- lec2.pdf;
-Slides: slide- lec3b.pptx;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 4, lectures- 1 Lecture, duration- 00:43;
-Video: link- https://drive.google.com/file/d/1JZjwQWO7_aTq04qMJLL5pf6HXNrv_qyN/preview, name- TPL Week#4, duration- 00:43;
-Topics: Compiler working flow chart, Top down parsing alogrithum, Construction of Syntaxtical Structure using BNF;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 6, lectures- 2 Lectures, duration- 01:42;
-Video: link- https://drive.google.com/file/d/1DJtOj-fOGE1gRrjlmTR0z7pvGFs5G7xU/preview, name- Part 1 Chapter 5 remaining, duration- 01:05;
-Video: link- https://drive.google.com/file/d/1aMmr-E7CAkgN8YMMwR4RX22u7qjPq6EH/preview, name- Part 2 Chapter 6 started, duration- 00:37;
-Topics: Variable life time, Variable scopes, Static Scope, Stack Dynamic scope, Explicit / implicit heap dynamic, Chapter 6 Introduction;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 1, lectures- 3 Lectures, duration- 01:47;
-Video: link- https://drive.google.com/file/d/1ctSBf7a08q8Au16-1HEayw8aghDsauQG/preview, name- TPL Week#1 Part1, duration- 00:17;
-Video: link- https://drive.google.com/file/d/17yY-6RGVlhAsfMqJVqewvXUHGmNDlcR1/preview, name- TPL Week#1 Part2, duration- 00:53;
-Slides: slide- Chapter 5.ppt;
-Books: name- Concepts of Programming Languages 11th Ed.pdf, link- Concepts of Programming Languages 11th Ed.pdf</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 2, lectures- 2 Lectures, duration- 01:40;
-Video: link- https://drive.google.com/file/d/15p5EP1_UCBHxyD9URakXw9xEW3hBKCLu/preview, name- TPL Week#2 Part 1, duration- 00:51;
-Video: link- https://drive.google.com/file/d/1hHFe7EcX_PNGHntkNqR0a4Q9tTmLY1d-/preview, name- TPL Week#2 Part 2, duration- 00:49;
-Slides: slide- Chapter 1.ppt;
-Slides: slide- Chapter 2.ppt;
-Slides: slide- Chapter 3.ppt;
-Topics: Readability, reliability, writeability, Chapter 3, Lexemes, Backus Naur Form (BNF), Parse Trees;
-Important: 1 question will come from Chapter 2;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 5, lectures- 1 Lecture, duration- 01:20;
-Video: link- https://drive.google.com/file/d/11P2oVuOQdNCB1lXC0azUnH74t3y6MwIx/preview, name- TPL Week#5, duration- 01:20;
-Slides: slide- Chapter 5.ppt;
-Topics: Context Free, Context Sensitive languages, Variable attributes, Possible binding times, Life time of a variable, Scope of a variable (example);</t>
-  </si>
-  <si>
-    <t>Topic: name- Mid Term Exam, lectures- , duration- 11 Nov | 15:00-16:30;
-Assignment: name- Past paper 2018, img- /TPL/pastpaper1.jpg*/TPL/pastpaper2.jpg;
-Slides: slide- Chapter 1.ppt;
-Slides: slide- Chapter 2.ppt;
-Slides: slide- Chapter 3.ppt;
-Slides: slide- Chapter 5.pptx;
-Books: name- Concepts of Programming Languages 11th Ed, link- Concepts of Programming Languages 11th Ed.pdf;
-Assignment: name- Mid Term Paper 2019, img- /TPL/mid20191.jpg*/TPL/mid20192.jpg;</t>
-  </si>
-  <si>
-    <t>Topic: name- Mid Term Exam, lectures- , duration- 12 Nov | 15:00-16:30;
-Assignment: name- Past Paper 2017, img- /SRE/mid exam past paper.jpeg;
-Slides: slide- Lecture Slide_1.pptx;
-Slides: slide- Lecture Slide_2.pptx;
-Slides: slide- Lecture Slide_3.pptx;
-Slides: slide- Lecture Slide_4.pptx;
-Books: name- Requirements Engineering Fundamentals, link- Requirements Engineering Fundamentals A Study Guide for the Certified Professional for Requirements Engineering Exam.pdf;
-Questions: Chapter 1, Goals of requirements engineering, Core activities of requirements engineering, Characteristics of requirements engineer, Requirements types, Categorization of Quality Requirements, Chapter 2, Aspects of system context, Sources and Sinks of a system, Documenting the system context, Chapter 3, Sources for elliciting requirements, Significance of stakeholders, Documenting stakeholders, Obligations of Requirements engineer, Previliges of stakeholders, Kano Model (Influence of requirements on sattisfaction), What influences selection of elicitation techniques, Human influences, Observation influence, Operational influence, Combining ellicitations techniques to lower risk, Interview, Questionaire, Creative techniques types, Brainstorming &amp; paradox, System archeology, Perspective based reading, Questions observation &amp; optimize process, Field observation, Apprenticing, Types of support techniques, Modelling action sequences, Chapter 4, Reason for documentations, Documentation Perspectives (Types), Advantages of using natural languages, 4 Conceptual Models, Standardized Structring Advantages, Names of different Standards (3), Parts of ISO 29148 Standard Document, Parts of Customized Standard Contents, Parts of introduction in custom standards, Parts of General Overview in Custom standards, Uses of requirements documents, Quality criteria for requirements documents;</t>
-  </si>
-  <si>
-    <t>IS</t>
-  </si>
-  <si>
-    <t>Subject: Special Topics in Information Security;
-Instructor: Dr Syed Nasir Mehmood Shah;
-ClassSenior: Waqas Wattoo | +92 301 3068788;
-Note: None yet;
-CreditHours: 3.0;</t>
-  </si>
-  <si>
-    <t>Topic: name- Course Material,lectures- 5 Lectures, duration- 00;
-Slides: slide- An Analysis of Security Threats in Cloud Computing.pptx;
-Slides: slide- Lecture1_Information Security.pdf;
-Slides: slide- Lecture2_SecureCloudFramework.pdf;
-Slides: slide- Lecture3_EmergingTrendsinCloudSecurity.pdf;
-Slides: slide- Muhammad Sadiq Thesis v1.7.pdf;</t>
+Books: name- Engineering &amp; Managing Software Requirements by Ayubuke Aurum &amp; Class Wohlin;
+Assignment: name- Assignment No 1, link- Assignment No.1 2.pdf;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 7, lectures- No lecture, duration- 00;
+Assignment: name- Assignment no 2, link- Assignment2.pdf;
+Note: heading- Note, text- No lecture conducted during this week due to exam on 17 Nov 2019. Sir only gave above assignment;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 7, lectures- No lecture, duration- 00;
+Assignment: name- Assignment no 2, img- /TPL/Assignment2.jpeg*/TPL/mid20191.jpg*/TPL/mid20192.jpg;
+Note: heading- Note, text- No lecture conducted during this week due to exam on 17 Nov 2019. Sir only gave above assignment.;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 8, lectures- , duration- ?;
+Note: heading- Note, text- Lecture not uploaded on google drive yet.</t>
   </si>
 </sst>
 </file>
@@ -821,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB8366-CFB7-BD41-BAF1-2BC53FC93C19}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -852,7 +866,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G1" s="12"/>
       <c r="N1" s="6"/>
@@ -863,36 +877,36 @@
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="14" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G2" s="12"/>
       <c r="N2" s="6"/>
     </row>
-    <row r="3" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>43720</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G3" s="12"/>
       <c r="N3" s="6"/>
@@ -903,13 +917,13 @@
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="12"/>
@@ -921,13 +935,13 @@
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N5" s="5"/>
     </row>
@@ -937,13 +951,13 @@
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="14" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>31</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="N6" s="5"/>
     </row>
@@ -953,13 +967,13 @@
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
@@ -971,13 +985,13 @@
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F8" s="10"/>
     </row>
@@ -987,30 +1001,36 @@
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="14" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="221" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+      <c r="C10" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>57</v>
+      </c>
       <c r="E10" s="14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+      <c r="E11" s="9" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>

</xml_diff>

<commit_message>
added request for donation
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46AC6509-168B-C744-9FF0-35C8DD59F753}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B15B8CF-39C4-A94B-9B89-1F86D992F647}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
@@ -418,7 +418,7 @@
   </si>
   <si>
     <t>Topic: name- Week 8, lectures- , duration- ?;
-Note: heading- Note, text- Lecture not uploaded on google drive yet.</t>
+Note: heading- Note, text- Lecture not uploaded on google drive yet. Kamran | 0302 5003156‬ normally uploads these lectures.</t>
   </si>
 </sst>
 </file>
@@ -1023,7 +1023,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="5"/>

</xml_diff>

<commit_message>
SRE assignment 2 added
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B15B8CF-39C4-A94B-9B89-1F86D992F647}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7330A6-71C5-3548-8116-0C1CFACBE796}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
@@ -408,17 +408,18 @@
   </si>
   <si>
     <t>Topic: name- Week 7, lectures- No lecture, duration- 00;
-Assignment: name- Assignment no 2, link- Assignment2.pdf;
-Note: heading- Note, text- No lecture conducted during this week due to exam on 17 Nov 2019. Sir only gave above assignment;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 7, lectures- No lecture, duration- 00;
 Assignment: name- Assignment no 2, img- /TPL/Assignment2.jpeg*/TPL/mid20191.jpg*/TPL/mid20192.jpg;
 Note: heading- Note, text- No lecture conducted during this week due to exam on 17 Nov 2019. Sir only gave above assignment.;</t>
   </si>
   <si>
     <t>Topic: name- Week 8, lectures- , duration- ?;
 Note: heading- Note, text- Lecture not uploaded on google drive yet. Kamran | 0302 5003156‬ normally uploads these lectures.</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 7, lectures- No lecture, duration- 00;
+Assignment: name- Assignment no 2, link- Assignment2.pdf;
+Assignment: name- Assignment no 2 Solved by Qasim, link- Assignment 2 Solved.docx;
+Note: heading- Note, text- No lecture conducted during this week due to exam on 17 Nov 2019. Sir only gave above assignment;</t>
   </si>
 </sst>
 </file>
@@ -836,7 +837,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1014,10 +1015,10 @@
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>43</v>
@@ -1029,7 +1030,7 @@
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
solved assignment for tpl added, logo for assignments changed
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7330A6-71C5-3548-8116-0C1CFACBE796}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D616CF-64D6-6144-BEBC-B4E48ED06240}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
@@ -408,18 +408,20 @@
   </si>
   <si>
     <t>Topic: name- Week 7, lectures- No lecture, duration- 00;
-Assignment: name- Assignment no 2, img- /TPL/Assignment2.jpeg*/TPL/mid20191.jpg*/TPL/mid20192.jpg;
+Assignment: name- Assignment no 2 (Deadline 23 Nov), img- /TPL/Assignment2.jpeg*/TPL/mid20191.jpg*/TPL/mid20192.jpg;
+Assignment: name- Assignment no 2 Solved, link- Assignment 2 Solved.docx;
 Note: heading- Note, text- No lecture conducted during this week due to exam on 17 Nov 2019. Sir only gave above assignment.;</t>
   </si>
   <si>
+    <t>Topic: name- Week 7, lectures- No lecture, duration- 00;
+Assignment: name- Assignment no 2 (Deadline 23 Nov), link- Assignment2.pdf;
+Assignment: name- Assignment no 2 Solved, link- Assignment 2 Solved.docx;
+Note: heading- Note, text- No lecture conducted during this week due to exam on 17 Nov 2019. Sir only gave above assignment;</t>
+  </si>
+  <si>
     <t>Topic: name- Week 8, lectures- , duration- ?;
+Assignment: name- Assignment 2 (Deadline 22 Nov), img- /ALGO/Assignment 2.png*/ALGO/Assignment 2 DL.png;
 Note: heading- Note, text- Lecture not uploaded on google drive yet. Kamran | 0302 5003156‬ normally uploads these lectures.</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 7, lectures- No lecture, duration- 00;
-Assignment: name- Assignment no 2, link- Assignment2.pdf;
-Assignment: name- Assignment no 2 Solved by Qasim, link- Assignment 2 Solved.docx;
-Note: heading- Note, text- No lecture conducted during this week due to exam on 17 Nov 2019. Sir only gave above assignment;</t>
   </si>
 </sst>
 </file>
@@ -837,7 +839,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -996,7 +998,7 @@
       </c>
       <c r="F8" s="10"/>
     </row>
-    <row r="9" spans="1:14" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>43775</v>
       </c>
@@ -1018,19 +1020,19 @@
         <v>57</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="119" x14ac:dyDescent="0.2">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="9" t="s">
-        <v>58</v>
+      <c r="E11" s="14" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added book for SRE assignment
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D616CF-64D6-6144-BEBC-B4E48ED06240}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA892B5-C851-C942-8E9C-8F01D0B08043}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
+    <workbookView xWindow="8320" yWindow="460" windowWidth="13740" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -413,15 +413,16 @@
 Note: heading- Note, text- No lecture conducted during this week due to exam on 17 Nov 2019. Sir only gave above assignment.;</t>
   </si>
   <si>
+    <t>Topic: name- Week 8, lectures- , duration- ?;
+Assignment: name- Assignment 2 (Deadline 22 Nov), img- /ALGO/Assignment 2.png*/ALGO/Assignment 2 DL.png;
+Note: heading- Note, text- Lecture not uploaded on google drive yet. Kamran | 0302 5003156‬ normally uploads these lectures.</t>
+  </si>
+  <si>
     <t>Topic: name- Week 7, lectures- No lecture, duration- 00;
 Assignment: name- Assignment no 2 (Deadline 23 Nov), link- Assignment2.pdf;
 Assignment: name- Assignment no 2 Solved, link- Assignment 2 Solved.docx;
+Books: name- Engineering and Managing software requirements by Aybuke Aurum and Claes Wohlin, link- Engineering and Managing software requirements.pdf; 
 Note: heading- Note, text- No lecture conducted during this week due to exam on 17 Nov 2019. Sir only gave above assignment;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 8, lectures- , duration- ?;
-Assignment: name- Assignment 2 (Deadline 22 Nov), img- /ALGO/Assignment 2.png*/ALGO/Assignment 2 DL.png;
-Note: heading- Note, text- Lecture not uploaded on google drive yet. Kamran | 0302 5003156‬ normally uploads these lectures.</t>
   </si>
 </sst>
 </file>
@@ -838,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB8366-CFB7-BD41-BAF1-2BC53FC93C19}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -998,7 +999,7 @@
       </c>
       <c r="F8" s="10"/>
     </row>
-    <row r="9" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>43775</v>
       </c>
@@ -1020,7 +1021,7 @@
         <v>57</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>43</v>
@@ -1032,7 +1033,7 @@
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fixed note placement in SRE
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA892B5-C851-C942-8E9C-8F01D0B08043}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB07E18-86E2-984A-9E26-614401AC52C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8320" yWindow="460" windowWidth="13740" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
@@ -421,7 +421,7 @@
     <t>Topic: name- Week 7, lectures- No lecture, duration- 00;
 Assignment: name- Assignment no 2 (Deadline 23 Nov), link- Assignment2.pdf;
 Assignment: name- Assignment no 2 Solved, link- Assignment 2 Solved.docx;
-Books: name- Engineering and Managing software requirements by Aybuke Aurum and Claes Wohlin, link- Engineering and Managing software requirements.pdf; 
+Books: name- Engineering and Managing software requirements by Aybuke Aurum and Claes Wohlin, link- Engineering and Managing software requirements.pdf;
 Note: heading- Note, text- No lecture conducted during this week due to exam on 17 Nov 2019. Sir only gave above assignment;</t>
   </si>
 </sst>
@@ -839,7 +839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB8366-CFB7-BD41-BAF1-2BC53FC93C19}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added week 9 for algo
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB07E18-86E2-984A-9E26-614401AC52C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347FD965-9E53-8747-A2ED-A38742AFFDEF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8320" yWindow="460" windowWidth="13740" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="61">
   <si>
     <t>Algo</t>
   </si>
@@ -413,16 +413,25 @@
 Note: heading- Note, text- No lecture conducted during this week due to exam on 17 Nov 2019. Sir only gave above assignment.;</t>
   </si>
   <si>
-    <t>Topic: name- Week 8, lectures- , duration- ?;
-Assignment: name- Assignment 2 (Deadline 22 Nov), img- /ALGO/Assignment 2.png*/ALGO/Assignment 2 DL.png;
-Note: heading- Note, text- Lecture not uploaded on google drive yet. Kamran | 0302 5003156‬ normally uploads these lectures.</t>
-  </si>
-  <si>
     <t>Topic: name- Week 7, lectures- No lecture, duration- 00;
 Assignment: name- Assignment no 2 (Deadline 23 Nov), link- Assignment2.pdf;
 Assignment: name- Assignment no 2 Solved, link- Assignment 2 Solved.docx;
 Books: name- Engineering and Managing software requirements by Aybuke Aurum and Claes Wohlin, link- Engineering and Managing software requirements.pdf;
 Note: heading- Note, text- No lecture conducted during this week due to exam on 17 Nov 2019. Sir only gave above assignment;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 8, lectures- 2 Lectures, duration- 01:33;
+Assignment: name- Assignment 2 (Deadline 22 Nov), img- /ALGO/Assignment 2.png*/ALGO/Assignment 2 DL.png;
+Video: link- https://drive.google.com/file/d/1lpPNJAvs6WzQuJ6z0dhX96HCxnarShVs/preview, name- AD&amp;AA Week # 8 Part1.mp4, duration- 00:54;
+Video: link- https://drive.google.com/file/d/1A8aBmhTcErBz6hETG1YYLN-GMCLMZUSX/preview, name- AD&amp;AA Week # 8 Part2.mp4, duration- 00:39;
+Slides: slide- lec4.pptx;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 9, lectures- , duration- 00:00;
+Assignment: name- Assignment 3 (Deadline 29 Nov), img- /ALGO/Assignment 3.png;
+Slides: slide- lec5.ppt;
+Important: Quiz in next class from lecture 5 (above slides);
+Note: heading- Note, text- Video lectures not uploaded on google drive yet. If you want them faster please call Kamran (Abasyn) at 0302 5003156‬.;</t>
   </si>
 </sst>
 </file>
@@ -839,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB8366-CFB7-BD41-BAF1-2BC53FC93C19}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -999,7 +1008,7 @@
       </c>
       <c r="F8" s="10"/>
     </row>
-    <row r="9" spans="1:14" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>43775</v>
       </c>
@@ -1021,27 +1030,29 @@
         <v>57</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="119" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="238" x14ac:dyDescent="0.2">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="153" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="E12" s="14" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="8"/>

</xml_diff>

<commit_message>
added algo topics after watching video
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A303AE54-7BFB-194F-9D8D-81A434291071}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45A8928-7925-9D4A-BF6B-5AD8EE549C98}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -287,12 +287,6 @@
 Slides: slide- lec3b.pptx;</t>
   </si>
   <si>
-    <t>Topic: name- Week 7,lectures- 2 Lectures, duration- 01:41;
-Video: link- https://drive.google.com/file/d/1iN0XDjE-kn0od8h8e3azwQFUaFEwDKEt/preview, name- AD&amp;AA Week#7 Part 1.mp4, duration- 00:57;
-Video: link- https://drive.google.com/file/d/130Cyy5mWSzIPNuH8qWlAk8wQcO5H_7o4/preview, name- AD&amp;AA Week#7 Part 2.mp4, duration- 00:44;
-Slides: slide- lec4.pptx;</t>
-  </si>
-  <si>
     <t>Topic: name- Week 5,lectures- 2 Lectures, duration- 01:16;
 Video: link- https://drive.google.com/file/d/1t6VMFiI4610ULxoovPeFNuAnRKYwKosu/preview, name- AD&amp;AA Week#5 Part 1.mp4, duration- 00:25;
 Video: link- https://drive.google.com/file/d/1s_RbEVFMh9pGqPTkgfURH9Kx8nGcK3GI/preview, name- AD&amp;AA Week#5 Part 2.mp4, duration- 00:51;
@@ -420,13 +414,6 @@
 Note: heading- Note, text- No lecture conducted during this week due to exam on 17 Nov 2019. Sir only gave above assignment;</t>
   </si>
   <si>
-    <t>Topic: name- Week 8, lectures- 2 Lectures, duration- 01:33;
-Assignment: name- Assignment 2 (Deadline 22 Nov), img- /ALGO/Assignment 2.png*/ALGO/Assignment 2 DL.png;
-Video: link- https://drive.google.com/file/d/1lpPNJAvs6WzQuJ6z0dhX96HCxnarShVs/preview, name- AD&amp;AA Week # 8 Part1.mp4, duration- 00:54;
-Video: link- https://drive.google.com/file/d/1A8aBmhTcErBz6hETG1YYLN-GMCLMZUSX/preview, name- AD&amp;AA Week # 8 Part2.mp4, duration- 00:39;
-Slides: slide- lec4.pptx;</t>
-  </si>
-  <si>
     <t>Topic: name- Week 9, lectures- , duration- 00:00;
 Assignment: name- Assignment 3 (Deadline 29 Nov), img- /ALGO/Assignment 3.png;
 Slides: slide- lec5.ppt;
@@ -437,6 +424,21 @@
     <t>Topic: name- Week 8, lectures- , duration- 00;
 Assignment: name- Assignment no 3 (Deadline 15 Dec 2019), img- /TPL/Assignment No 3 TPL.png;
 Note: heading- Note, text- Video lectures not uploaded on google drive yet. If you want them faster please call Kamran (Abasyn) at 0302 5003156‬.;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 8, lectures- 2 Lectures, duration- 01:33;
+Assignment: name- Assignment 2 (Deadline 22 Nov), img- /ALGO/Assignment 2.png*/ALGO/Assignment 2 DL.png;
+Video: link- https://drive.google.com/file/d/1lpPNJAvs6WzQuJ6z0dhX96HCxnarShVs/preview, name- AD&amp;AA Week # 8 Part1.mp4, duration- 00:54;
+Video: link- https://drive.google.com/file/d/1A8aBmhTcErBz6hETG1YYLN-GMCLMZUSX/preview, name- AD&amp;AA Week # 8 Part2.mp4, duration- 00:39;
+Slides: slide- lec4.pptx;
+Topics: Redex Sort, Bubble Sort;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 7,lectures- 2 Lectures, duration- 01:41;
+Video: link- https://drive.google.com/file/d/1iN0XDjE-kn0od8h8e3azwQFUaFEwDKEt/preview, name- AD&amp;AA Week#7 Part 1.mp4, duration- 00:57;
+Video: link- https://drive.google.com/file/d/130Cyy5mWSzIPNuH8qWlAk8wQcO5H_7o4/preview, name- AD&amp;AA Week#7 Part 2.mp4, duration- 00:44;
+Slides: slide- lec4.pptx;
+Topics: Chapter 4, Effciency of Algorithum, Types of Algorithms in Relation to Time, Insertion Algorihum, Selection Algorithum, Shall Sort;</t>
   </si>
 </sst>
 </file>
@@ -853,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB8366-CFB7-BD41-BAF1-2BC53FC93C19}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -884,7 +886,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G1" s="12"/>
       <c r="N1" s="6"/>
@@ -895,16 +897,16 @@
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>54</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>55</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>36</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G2" s="12"/>
       <c r="N2" s="6"/>
@@ -915,16 +917,16 @@
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>35</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G3" s="12"/>
       <c r="N3" s="6"/>
@@ -935,7 +937,7 @@
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>29</v>
@@ -969,7 +971,7 @@
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>31</v>
@@ -985,13 +987,13 @@
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
@@ -1003,7 +1005,7 @@
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>37</v>
@@ -1019,37 +1021,37 @@
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="14" t="s">
-        <v>50</v>
-      </c>
       <c r="E9" s="14" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="221" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="14" t="s">
-        <v>58</v>
-      </c>
       <c r="E10" s="14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="238" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="255" x14ac:dyDescent="0.2">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="153" x14ac:dyDescent="0.2">
@@ -1058,7 +1060,7 @@
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
week 8 and 9 updated
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45A8928-7925-9D4A-BF6B-5AD8EE549C98}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F3281E-72D2-AB48-9FD6-29807E79813F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="63">
   <si>
     <t>Algo</t>
   </si>
@@ -381,13 +381,6 @@
 CreditHours: 3.0;</t>
   </si>
   <si>
-    <t>Subject: Software Requirement Engineering;
-Instructor: Mr Fazal Wahab;
-ClassSenior: Fakhar | +92 ‭332 0278998‬;
-Note: No lecture on 16 Nov due to papers;
-CreditHours: 3.0;</t>
-  </si>
-  <si>
     <t>Topic: name- Week 1,lectures- 3 Lectures, duration- 01:47;
 Video: link- https://drive.google.com/file/d/1brUQVmv6OGb2n1GePe4c5fjrVbVJUFvz/preview, name- Class CR Number, duration- 00:04;
 Video: link- https://drive.google.com/file/d/1-oeLFxAxdOeAgkILn1uyLbTcr-NsZlIT/preview, name- SRE Week#1 Part1.mp4, duration- 56:47;
@@ -401,44 +394,59 @@
 Assignment: name- Assignment No 1, link- Assignment No.1 2.pdf;</t>
   </si>
   <si>
-    <t>Topic: name- Week 7, lectures- No lecture, duration- 00;
-Assignment: name- Assignment no 2 (Deadline 23 Nov), img- /TPL/Assignment2.jpeg*/TPL/mid20191.jpg*/TPL/mid20192.jpg;
-Assignment: name- Assignment no 2 Solved, link- Assignment 2 Solved.docx;
-Note: heading- Note, text- No lecture conducted during this week due to exam on 17 Nov 2019. Sir only gave above assignment.;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 7, lectures- No lecture, duration- 00;
-Assignment: name- Assignment no 2 (Deadline 23 Nov), link- Assignment2.pdf;
-Assignment: name- Assignment no 2 Solved, link- Assignment 2 Solved.docx;
-Books: name- Engineering and Managing software requirements by Aybuke Aurum and Claes Wohlin, link- Engineering and Managing software requirements.pdf;
-Note: heading- Note, text- No lecture conducted during this week due to exam on 17 Nov 2019. Sir only gave above assignment;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 9, lectures- , duration- 00:00;
-Assignment: name- Assignment 3 (Deadline 29 Nov), img- /ALGO/Assignment 3.png;
-Slides: slide- lec5.ppt;
-Important: Quiz in next class from lecture 5 (above slides);
-Note: heading- Note, text- Video lectures not uploaded on google drive yet. If you want them faster please call Kamran (Abasyn) at 0302 5003156‬.;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 8, lectures- , duration- 00;
-Assignment: name- Assignment no 3 (Deadline 15 Dec 2019), img- /TPL/Assignment No 3 TPL.png;
-Note: heading- Note, text- Video lectures not uploaded on google drive yet. If you want them faster please call Kamran (Abasyn) at 0302 5003156‬.;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 8, lectures- 2 Lectures, duration- 01:33;
-Assignment: name- Assignment 2 (Deadline 22 Nov), img- /ALGO/Assignment 2.png*/ALGO/Assignment 2 DL.png;
-Video: link- https://drive.google.com/file/d/1lpPNJAvs6WzQuJ6z0dhX96HCxnarShVs/preview, name- AD&amp;AA Week # 8 Part1.mp4, duration- 00:54;
-Video: link- https://drive.google.com/file/d/1A8aBmhTcErBz6hETG1YYLN-GMCLMZUSX/preview, name- AD&amp;AA Week # 8 Part2.mp4, duration- 00:39;
-Slides: slide- lec4.pptx;
-Topics: Redex Sort, Bubble Sort;</t>
-  </si>
-  <si>
     <t>Topic: name- Week 7,lectures- 2 Lectures, duration- 01:41;
 Video: link- https://drive.google.com/file/d/1iN0XDjE-kn0od8h8e3azwQFUaFEwDKEt/preview, name- AD&amp;AA Week#7 Part 1.mp4, duration- 00:57;
 Video: link- https://drive.google.com/file/d/130Cyy5mWSzIPNuH8qWlAk8wQcO5H_7o4/preview, name- AD&amp;AA Week#7 Part 2.mp4, duration- 00:44;
 Slides: slide- lec4.pptx;
 Topics: Chapter 4, Effciency of Algorithum, Types of Algorithms in Relation to Time, Insertion Algorihum, Selection Algorithum, Shall Sort;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 8, lectures- 2 Lectures, duration- 01:33;
+Video: link- https://drive.google.com/file/d/1lpPNJAvs6WzQuJ6z0dhX96HCxnarShVs/preview, name- AD&amp;AA Week # 8 Part1.mp4, duration- 00:54;
+Video: link- https://drive.google.com/file/d/1A8aBmhTcErBz6hETG1YYLN-GMCLMZUSX/preview, name- AD&amp;AA Week # 8 Part2.mp4, duration- 00:39;
+Assignment: name- Assignment 2 (Deadline 22 Nov), img- /ALGO/Assignment 2.png*/ALGO/Assignment 2 DL.png;
+Slides: slide- lec4.pptx;
+Topics: Redex Sort, Bubble Sort;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 9, lectures- 2 Lectures, duration- 01:51;
+Video: link- https://drive.google.com/file/d/1430C-n3l2kRoy2Qn76kBep_umfClXmkF/preview, name- AD&amp;AA Week # 9 Part1.mp4, duration- 00:38;
+Video: link- https://drive.google.com/file/d/1UBidBALGcA7KB8t11RDEwlTti64BilJf/preview, name- AD&amp;AA Week # 9 Part2.mp4, duration- 01:13;
+Assignment: name- Assignment 3 (Deadline 29 Nov), img- /ALGO/Assignment 3.png;
+Slides: slide- lec5.ppt;
+Important: Quiz in next class from lecture 5 (above slides);</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 8, lectures- 3 Lectures, duration- 01:22;
+Video: link- https://drive.google.com/file/d/18sP4Wf0WZh_3gh0PCDZaPH0YT7HsDmhn/preview, name- SRE Week8 Part#1.mp4, duration- 00:01;
+Video: link- https://drive.google.com/file/d/1cFUxdRC5VwlsjxILvMbMqO6SVWkXwZB1/preview, name- SRE Week8 Part#2.mp4, duration- 00:51;
+Video: link- https://drive.google.com/file/d/128EIgEoYNkqrN_PCG30nwpn1MGaNhK-J/preview, name- SRE Week8 Part#3.mp4, duration- 00:30;
+Assignment: name- Assignment no 3 (Deadline 21 Dec 2019), img- /SRE/Assignment 3.png;</t>
+  </si>
+  <si>
+    <t>Subject: Software Requirement Engineering;
+Instructor: Mr Fazal Wahab;
+ClassSenior: Fakhar | +92 ‭332 0278998‬;
+Note: From this Saturday (30 Nov 2019) to end of semester means four weeks, there will extra 1 and half hour makeup class of SRE after maghrib prayer.;
+CreditHours: 3.0;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 8, lectures- , duration- ;
+Assignment: name- Assignment no 3 (Deadline 15 Dec 2019), img- /TPL/Assignment No 3 TPL.png;
+Note: heading- Note, text- Video lectures not uploaded on google drive yet. If you want them faster please call Kamran (Abasyn) at 0302 5003156‬.;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 7, lectures- Assignment Only, duration- ;
+Assignment: name- Assignment no 2 (Deadline 23 Nov), img- /TPL/Assignment2.jpeg*/TPL/mid20191.jpg*/TPL/mid20192.jpg;
+Assignment: name- Assignment no 2 Solved, link- Assignment 2 Solved.docx;
+Note: heading- Note, text- No lecture conducted during this week due to exam on 17 Nov 2019. Sir only gave above assignment.;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 7, lectures- Assignment Only, duration- ;
+Assignment: name- Assignment no 2 (Deadline 23 Nov), link- Assignment2.pdf;
+Assignment: name- Assignment no 2 Solved, link- Assignment 2 Solved.docx;
+Books: name- Engineering and Managing software requirements by Aybuke Aurum and Claes Wohlin, link- Engineering and Managing software requirements.pdf;
+Note: heading- Note, text- No lecture conducted during this week due to exam on 17 Nov 2019. Sir only gave above assignment;</t>
   </si>
 </sst>
 </file>
@@ -855,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB8366-CFB7-BD41-BAF1-2BC53FC93C19}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -891,7 +899,7 @@
       <c r="G1" s="12"/>
       <c r="N1" s="6"/>
     </row>
-    <row r="2" spans="1:14" ht="102" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="119" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
@@ -900,7 +908,7 @@
         <v>53</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>36</v>
@@ -920,7 +928,7 @@
         <v>45</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>35</v>
@@ -1015,7 +1023,7 @@
       </c>
       <c r="F8" s="10"/>
     </row>
-    <row r="9" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>43775</v>
       </c>
@@ -1027,17 +1035,17 @@
         <v>49</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="221" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="14" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>42</v>
@@ -1047,20 +1055,22 @@
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="5"/>
+        <v>60</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>58</v>
+      </c>
       <c r="E11" s="14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="153" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="238" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
week 9 all subjects added
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F3281E-72D2-AB48-9FD6-29807E79813F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B45B224-D1DD-6048-A9A1-98D0026DA5B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="66">
   <si>
     <t>Algo</t>
   </si>
@@ -302,11 +302,6 @@
 Slides: slide- lec3b.pptx;</t>
   </si>
   <si>
-    <t>Topic: name- Week 4, lectures- 1 Lecture, duration- 00:43;
-Video: link- https://drive.google.com/file/d/1JZjwQWO7_aTq04qMJLL5pf6HXNrv_qyN/preview, name- TPL Week#4, duration- 00:43;
-Topics: Compiler working flow chart, Top down parsing alogrithum, Construction of Syntaxtical Structure using BNF;</t>
-  </si>
-  <si>
     <t>Topic: name- Week 6, lectures- 2 Lectures, duration- 01:42;
 Video: link- https://drive.google.com/file/d/1DJtOj-fOGE1gRrjlmTR0z7pvGFs5G7xU/preview, name- Part 1 Chapter 5 remaining, duration- 01:05;
 Video: link- https://drive.google.com/file/d/1aMmr-E7CAkgN8YMMwR4RX22u7qjPq6EH/preview, name- Part 2 Chapter 6 started, duration- 00:37;
@@ -401,29 +396,6 @@
 Topics: Chapter 4, Effciency of Algorithum, Types of Algorithms in Relation to Time, Insertion Algorihum, Selection Algorithum, Shall Sort;</t>
   </si>
   <si>
-    <t>Topic: name- Week 8, lectures- 2 Lectures, duration- 01:33;
-Video: link- https://drive.google.com/file/d/1lpPNJAvs6WzQuJ6z0dhX96HCxnarShVs/preview, name- AD&amp;AA Week # 8 Part1.mp4, duration- 00:54;
-Video: link- https://drive.google.com/file/d/1A8aBmhTcErBz6hETG1YYLN-GMCLMZUSX/preview, name- AD&amp;AA Week # 8 Part2.mp4, duration- 00:39;
-Assignment: name- Assignment 2 (Deadline 22 Nov), img- /ALGO/Assignment 2.png*/ALGO/Assignment 2 DL.png;
-Slides: slide- lec4.pptx;
-Topics: Redex Sort, Bubble Sort;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 9, lectures- 2 Lectures, duration- 01:51;
-Video: link- https://drive.google.com/file/d/1430C-n3l2kRoy2Qn76kBep_umfClXmkF/preview, name- AD&amp;AA Week # 9 Part1.mp4, duration- 00:38;
-Video: link- https://drive.google.com/file/d/1UBidBALGcA7KB8t11RDEwlTti64BilJf/preview, name- AD&amp;AA Week # 9 Part2.mp4, duration- 01:13;
-Assignment: name- Assignment 3 (Deadline 29 Nov), img- /ALGO/Assignment 3.png;
-Slides: slide- lec5.ppt;
-Important: Quiz in next class from lecture 5 (above slides);</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 8, lectures- 3 Lectures, duration- 01:22;
-Video: link- https://drive.google.com/file/d/18sP4Wf0WZh_3gh0PCDZaPH0YT7HsDmhn/preview, name- SRE Week8 Part#1.mp4, duration- 00:01;
-Video: link- https://drive.google.com/file/d/1cFUxdRC5VwlsjxILvMbMqO6SVWkXwZB1/preview, name- SRE Week8 Part#2.mp4, duration- 00:51;
-Video: link- https://drive.google.com/file/d/128EIgEoYNkqrN_PCG30nwpn1MGaNhK-J/preview, name- SRE Week8 Part#3.mp4, duration- 00:30;
-Assignment: name- Assignment no 3 (Deadline 21 Dec 2019), img- /SRE/Assignment 3.png;</t>
-  </si>
-  <si>
     <t>Subject: Software Requirement Engineering;
 Instructor: Mr Fazal Wahab;
 ClassSenior: Fakhar | +92 ‭332 0278998‬;
@@ -431,11 +403,6 @@
 CreditHours: 3.0;</t>
   </si>
   <si>
-    <t>Topic: name- Week 8, lectures- , duration- ;
-Assignment: name- Assignment no 3 (Deadline 15 Dec 2019), img- /TPL/Assignment No 3 TPL.png;
-Note: heading- Note, text- Video lectures not uploaded on google drive yet. If you want them faster please call Kamran (Abasyn) at 0302 5003156‬.;</t>
-  </si>
-  <si>
     <t>Topic: name- Week 7, lectures- Assignment Only, duration- ;
 Assignment: name- Assignment no 2 (Deadline 23 Nov), img- /TPL/Assignment2.jpeg*/TPL/mid20191.jpg*/TPL/mid20192.jpg;
 Assignment: name- Assignment no 2 Solved, link- Assignment 2 Solved.docx;
@@ -447,6 +414,60 @@
 Assignment: name- Assignment no 2 Solved, link- Assignment 2 Solved.docx;
 Books: name- Engineering and Managing software requirements by Aybuke Aurum and Claes Wohlin, link- Engineering and Managing software requirements.pdf;
 Note: heading- Note, text- No lecture conducted during this week due to exam on 17 Nov 2019. Sir only gave above assignment;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 8, lectures- , duration- ;
+Slides: slide- Chapter 6.ppt;
+Assignment: name- Assignment no 3 (Deadline 15 Dec 2019), img- /TPL/Assignment No 3 TPL.png;
+Note: heading- Note, text- Video lectures not uploaded on google drive yet. If you want them faster please call Kamran (Abasyn) at 0302 5003156‬.;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 4, lectures- 1 Lecture, duration- 00:43;
+Video: link- https://drive.google.com/file/d/1JZjwQWO7_aTq04qMJLL5pf6HXNrv_qyN/preview, name- TPL Week#4, duration- 00:43;
+Slides: slide- Chapter 4.ppt;
+Topics: Compiler working flow chart, Top down parsing alogrithum, Construction of Syntaxtical Structure using BNF;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 8, lectures- 3 Lectures, duration- 01:22;
+Video: link- https://drive.google.com/file/d/18sP4Wf0WZh_3gh0PCDZaPH0YT7HsDmhn/preview, name- SRE Week8 Part#1.mp4, duration- 00:01;
+Video: link- https://drive.google.com/file/d/1cFUxdRC5VwlsjxILvMbMqO6SVWkXwZB1/preview, name- SRE Week8 Part#2.mp4, duration- 00:51;
+Video: link- https://drive.google.com/file/d/128EIgEoYNkqrN_PCG30nwpn1MGaNhK-J/preview, name- SRE Week8 Part#3.mp4, duration- 00:30;
+Assignment: name- Assignment no 3 (Deadline 21 Dec 2019), img- /SRE/Assignment 3.png;
+Slides: slide- Lecture Slide_5.pptx;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 10, lectures- , duration- ;
+Slides: slide- Lec6.pptx;
+Note: heading- Video lectures not uploaded yet;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 9, lectures- , duration- ;
+Slides: slide- Lecture Slide_5.pptx;
+Important: Quiz from Lecture 5 (above lecture) in next class. Please come prepared.;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 9, lectures- , duration- ;
+Slides: slide- Chapter 6.ppt;
+Note: heading- Note, text- Video lectures not uploaded on google drive yet. If you want them faster please call Kamran (Abasyn) at 0302 5003156‬.;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 8, lectures- 2 Lectures, duration- 01:33;
+Video: link- https://drive.google.com/file/d/1lpPNJAvs6WzQuJ6z0dhX96HCxnarShVs/preview, name- AD&amp;AA Week # 8 Part1.mp4, duration- 00:54;
+Video: link- https://drive.google.com/file/d/1A8aBmhTcErBz6hETG1YYLN-GMCLMZUSX/preview, name- AD&amp;AA Week # 8 Part2.mp4, duration- 00:39;
+Assignment: name- Assignment 2 (Deadline 22 Nov), img- /ALGO/Assignment 2.png*/ALGO/Assignment 2 DL.png;
+Assignment: name- Assignment 2 Solved, img- /ALGO/Assignment20.jpg*/ALGO/Assignment21.jpg;
+Slides: slide- lec4.pptx;
+Topics: Redex Sort, Bubble Sort, Merge Sort, Counting Sort, Bucket Sort;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 9, lectures- 2 Lectures, duration- 01:51;
+Video: link- https://drive.google.com/file/d/1430C-n3l2kRoy2Qn76kBep_umfClXmkF/preview, name- AD&amp;AA Week # 9 Part1.mp4, duration- 00:38;
+Video: link- https://drive.google.com/file/d/1UBidBALGcA7KB8t11RDEwlTti64BilJf/preview, name- AD&amp;AA Week # 9 Part2.mp4, duration- 01:13;
+Assignment: name- Assignment 3 (Deadline 29 Nov), img- /ALGO/Assignment 3.png;
+Assignment: name- Assignment 3 Solved, img- /ALGO/Assignment30.jpg*/ALGO/Assignment31.jpg;
+Slides: slide- lec5.ppt;
+Important: Quiz in next class from lecture 5 (above slides);
+Topics: Pigeon hole sort, Important points for algorithms, Chapter 5, Asymptotatic analysis, Rate of growth, Wilson, Fibonacci, Investing on algorithms or computing?;</t>
   </si>
 </sst>
 </file>
@@ -863,8 +884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB8366-CFB7-BD41-BAF1-2BC53FC93C19}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -894,7 +915,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G1" s="12"/>
       <c r="N1" s="6"/>
@@ -905,16 +926,16 @@
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>36</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G2" s="12"/>
       <c r="N2" s="6"/>
@@ -925,16 +946,16 @@
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>35</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G3" s="12"/>
       <c r="N3" s="6"/>
@@ -945,7 +966,7 @@
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>29</v>
@@ -979,7 +1000,7 @@
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="14" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>31</v>
@@ -995,7 +1016,7 @@
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>30</v>
@@ -1013,7 +1034,7 @@
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>37</v>
@@ -1029,56 +1050,62 @@
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="14" t="s">
-        <v>49</v>
-      </c>
       <c r="E9" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="221" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="14" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="255" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="306" x14ac:dyDescent="0.2">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="14" t="s">
-        <v>58</v>
-      </c>
       <c r="E11" s="14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="238" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="323" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+      <c r="C12" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>62</v>
+      </c>
       <c r="E12" s="14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="E13" s="14" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>

</xml_diff>

<commit_message>
added mid result for algo
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B45B224-D1DD-6048-A9A1-98D0026DA5B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB28AC67-5AB0-EC46-8591-C73F11B13109}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
@@ -293,15 +293,6 @@
 Slides: slide- lec3a.ppt</t>
   </si>
   <si>
-    <t>Topic: name- Mid Term Exam, lectures- , duration- 8 Nov | 16:00-17:30;
-Assignment: name- Mid Term Exam Pattern, img- /ALGO/paperpattern.png;
-Assignment: name- Past Paper Mid Term (2018), img- /ALGO/quiz2018.jpg;
-Assignment: name- Solution of Past Paper, img- /ALGO/mid2018soln1.png*/ALGO/mid2018soln1b.jpg*/ALGO/mid2018soln2.png*/ALGO/mid2018soln3a.jpg*/ALGO/mid2018soln3b.jpg*/ALGO/mid2018soln3c.jpg;
-Slides: slide- lec1.pptx;
-Slides: slide- lec2.pdf;
-Slides: slide- lec3b.pptx;</t>
-  </si>
-  <si>
     <t>Topic: name- Week 6, lectures- 2 Lectures, duration- 01:42;
 Video: link- https://drive.google.com/file/d/1DJtOj-fOGE1gRrjlmTR0z7pvGFs5G7xU/preview, name- Part 1 Chapter 5 remaining, duration- 01:05;
 Video: link- https://drive.google.com/file/d/1aMmr-E7CAkgN8YMMwR4RX22u7qjPq6EH/preview, name- Part 2 Chapter 6 started, duration- 00:37;
@@ -468,6 +459,16 @@
 Slides: slide- lec5.ppt;
 Important: Quiz in next class from lecture 5 (above slides);
 Topics: Pigeon hole sort, Important points for algorithms, Chapter 5, Asymptotatic analysis, Rate of growth, Wilson, Fibonacci, Investing on algorithms or computing?;</t>
+  </si>
+  <si>
+    <t>Topic: name- Mid Term Exam, lectures- , duration- 8 Nov | 16:00-17:30;
+Assignment: name- Mid Term Exam Pattern, img- /ALGO/paperpattern.png;
+Assignment: name- Past Paper Mid Term (2018), img- /ALGO/quiz2018.jpg;
+Assignment: name- Solution of Past Paper, img- /ALGO/mid2018soln1.png*/ALGO/mid2018soln1b.jpg*/ALGO/mid2018soln2.png*/ALGO/mid2018soln3a.jpg*/ALGO/mid2018soln3b.jpg*/ALGO/mid2018soln3c.jpg;
+Slides: slide- lec1.pptx;
+Slides: slide- lec2.pdf;
+Slides: slide- lec3b.pptx;
+Slides: slide- Algo mid result.xlsx;</t>
   </si>
 </sst>
 </file>
@@ -884,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB8366-CFB7-BD41-BAF1-2BC53FC93C19}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -915,7 +916,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G1" s="12"/>
       <c r="N1" s="6"/>
@@ -926,16 +927,16 @@
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>36</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G2" s="12"/>
       <c r="N2" s="6"/>
@@ -946,16 +947,16 @@
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>35</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G3" s="12"/>
       <c r="N3" s="6"/>
@@ -966,7 +967,7 @@
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>29</v>
@@ -1000,7 +1001,7 @@
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>31</v>
@@ -1016,7 +1017,7 @@
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>30</v>
@@ -1034,7 +1035,7 @@
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>37</v>
@@ -1050,52 +1051,52 @@
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="14" t="s">
-        <v>48</v>
-      </c>
       <c r="E9" s="14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="221" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="238" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="14" t="s">
-        <v>57</v>
-      </c>
       <c r="E10" s="14" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="306" x14ac:dyDescent="0.2">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="323" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="51" x14ac:dyDescent="0.2">
@@ -1104,7 +1105,7 @@
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
till week 11 updated
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB28AC67-5AB0-EC46-8591-C73F11B13109}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CEF9E15-BF5D-C34B-B113-948C227D1885}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="70">
   <si>
     <t>Algo</t>
   </si>
@@ -395,22 +395,10 @@
   </si>
   <si>
     <t>Topic: name- Week 7, lectures- Assignment Only, duration- ;
-Assignment: name- Assignment no 2 (Deadline 23 Nov), img- /TPL/Assignment2.jpeg*/TPL/mid20191.jpg*/TPL/mid20192.jpg;
-Assignment: name- Assignment no 2 Solved, link- Assignment 2 Solved.docx;
-Note: heading- Note, text- No lecture conducted during this week due to exam on 17 Nov 2019. Sir only gave above assignment.;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 7, lectures- Assignment Only, duration- ;
 Assignment: name- Assignment no 2 (Deadline 23 Nov), link- Assignment2.pdf;
 Assignment: name- Assignment no 2 Solved, link- Assignment 2 Solved.docx;
 Books: name- Engineering and Managing software requirements by Aybuke Aurum and Claes Wohlin, link- Engineering and Managing software requirements.pdf;
 Note: heading- Note, text- No lecture conducted during this week due to exam on 17 Nov 2019. Sir only gave above assignment;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 8, lectures- , duration- ;
-Slides: slide- Chapter 6.ppt;
-Assignment: name- Assignment no 3 (Deadline 15 Dec 2019), img- /TPL/Assignment No 3 TPL.png;
-Note: heading- Note, text- Video lectures not uploaded on google drive yet. If you want them faster please call Kamran (Abasyn) at 0302 5003156‬.;</t>
   </si>
   <si>
     <t>Topic: name- Week 4, lectures- 1 Lecture, duration- 00:43;
@@ -425,21 +413,6 @@
 Video: link- https://drive.google.com/file/d/128EIgEoYNkqrN_PCG30nwpn1MGaNhK-J/preview, name- SRE Week8 Part#3.mp4, duration- 00:30;
 Assignment: name- Assignment no 3 (Deadline 21 Dec 2019), img- /SRE/Assignment 3.png;
 Slides: slide- Lecture Slide_5.pptx;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 10, lectures- , duration- ;
-Slides: slide- Lec6.pptx;
-Note: heading- Video lectures not uploaded yet;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 9, lectures- , duration- ;
-Slides: slide- Lecture Slide_5.pptx;
-Important: Quiz from Lecture 5 (above lecture) in next class. Please come prepared.;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 9, lectures- , duration- ;
-Slides: slide- Chapter 6.ppt;
-Note: heading- Note, text- Video lectures not uploaded on google drive yet. If you want them faster please call Kamran (Abasyn) at 0302 5003156‬.;</t>
   </si>
   <si>
     <t>Topic: name- Week 8, lectures- 2 Lectures, duration- 01:33;
@@ -469,6 +442,53 @@
 Slides: slide- lec2.pdf;
 Slides: slide- lec3b.pptx;
 Slides: slide- Algo mid result.xlsx;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 9, lectures- 2 Lectures, duration- 01:27;
+Video: link- https://drive.google.com/file/d/1mAiv1VBzdv_iIIRzMaK5Dgpn-_uW-qDG/preview, name- SRE Week # 9 Part 1.mp4, duration- 00:43;
+Video: link- https://drive.google.com/file/d/1HsNdz2rcUllt2Gx-qJXpnS653p8WA42G/preview, name- SRE Week # 9 Part 2.mp4, duration- 00:44;
+Slides: slide- Lecture Slide_5.pptx;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 10, lectures- 2 Lectures, duration- 01:24;
+Video: link- https://drive.google.com/file/d/1dy930AUWj6FhpQW_GAbGijpuZLD7owMZ/preview, name- AD&amp;AA Week # 10 Part 1.mp4, duration- 00:54;
+Video: link- https://drive.google.com/file/d/1Yz6n4GBQL6TryaLlmySsDhCP9y4XplkR/preview, name- AD&amp;AA Week # 10 Part 2.mp4, duration- 00:30;
+Slides: slide- Lec6.pptx;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 11, lectures- 2 Lectures, duration- 01:18;
+Video: link- https://drive.google.com/file/d/1L8AXlWHcUH16jcl_Zu8UyUj6iwnvuCx-/preview, name- AD&amp;AA Week # 11 Part 1.mp4, duration- 00:52;
+Video: link- https://drive.google.com/file/d/1ba5ptKIgEeli77GEPoVeP-v6XeBzV_nU/preview, name- AD&amp;AA Week # 11 Part 2.mp4, duration- 00:26;
+Assignment: name- Assignment 4, img- /ALGO/Assignment 4.png;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 8, lectures- 1 Lecture, duration- 01:26;
+Video: link- https://drive.google.com/file/d/1Uc4upqacrhA2-FtxU8GKFDuNC_Mw8Pmz/preview, name- TPL Week # 8.mp4, duration- 01:26;
+Slides: slide- Chapter 6.ppt;
+Assignment: name- Assignment no 3 (Deadline 15 Dec 2019), img- /TPL/Assignment No 3 TPL.png;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 7, lectures- Assignment Only, duration- -;
+Assignment: name- Assignment no 2 (Deadline 23 Nov), img- /TPL/Assignment2.jpeg*/TPL/mid20191.jpg*/TPL/mid20192.jpg;
+Assignment: name- Assignment no 2 Solved, link- Assignment 2 Solved.docx;
+Note: heading- Note, text- No lecture conducted during this week due to exam on 17 Nov 2019. Sir only gave above assignment.;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 10, lectures- Not uploaded, duration- -;
+Note: heading- Lectures not uploaded yet;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 11, lectures- Not uploaded, duration- -;
+Note: heading- Lectures not uploaded yet;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 9, lectures- Not uploaded, duration- -;
+Note: heading- Lectures not uploaded yet;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 11, lectures- Assignment Only, duration- -;
+Slides: slide- Chapter 7.ppt;
+Assignment: name- Quiz in next class from above Chapter 7, img- /TPL/Assignment 4.png;</t>
   </si>
 </sst>
 </file>
@@ -885,8 +905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB8366-CFB7-BD41-BAF1-2BC53FC93C19}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1001,7 +1021,7 @@
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>31</v>
@@ -1064,56 +1084,66 @@
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="14" t="s">
-        <v>56</v>
-      </c>
       <c r="E10" s="14" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="306" x14ac:dyDescent="0.2">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="14" t="s">
-        <v>59</v>
-      </c>
       <c r="E11" s="14" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="323" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="14" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>61</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="187" x14ac:dyDescent="0.2">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+      <c r="C13" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>66</v>
+      </c>
       <c r="E13" s="14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="204" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="C14" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="8"/>

</xml_diff>

<commit_message>
added lecture for SRE
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CEF9E15-BF5D-C34B-B113-948C227D1885}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CF2BB0-D16C-0F4D-AD1A-AD9A2FE4B6A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="71">
   <si>
     <t>Algo</t>
   </si>
@@ -489,6 +489,11 @@
     <t>Topic: name- Week 11, lectures- Assignment Only, duration- -;
 Slides: slide- Chapter 7.ppt;
 Assignment: name- Quiz in next class from above Chapter 7, img- /TPL/Assignment 4.png;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 10, lectures- 2 Lectures, duration- 01:19;
+Video: link- https://drive.google.com/file/d/1hrYmZgBA3wWiNbPf_0y_EjNAqVAep68S/preview, name- SRE Week # 10 Part 1.mp4, duration- 00:47;
+Video: link- https://drive.google.com/file/d/1C04hEIeBg2hEUmLco-5QQbT3AWkTYPIz/preview, name- SRE Week # 10 Part 2.mp4, duration- 00:32;</t>
   </si>
 </sst>
 </file>
@@ -905,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB8366-CFB7-BD41-BAF1-2BC53FC93C19}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1126,7 +1131,7 @@
         <v>66</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E13" s="14" t="s">
         <v>62</v>

</xml_diff>

<commit_message>
after mids syllabus added for algo
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/QasimAli/nodejs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CF2BB0-D16C-0F4D-AD1A-AD9A2FE4B6A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB1614F-1A58-8140-B755-573824946309}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="18580" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="74">
   <si>
     <t>Algo</t>
   </si>
@@ -478,14 +478,6 @@
 Note: heading- Lectures not uploaded yet;</t>
   </si>
   <si>
-    <t>Topic: name- Week 11, lectures- Not uploaded, duration- -;
-Note: heading- Lectures not uploaded yet;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 9, lectures- Not uploaded, duration- -;
-Note: heading- Lectures not uploaded yet;</t>
-  </si>
-  <si>
     <t>Topic: name- Week 11, lectures- Assignment Only, duration- -;
 Slides: slide- Chapter 7.ppt;
 Assignment: name- Quiz in next class from above Chapter 7, img- /TPL/Assignment 4.png;</t>
@@ -494,6 +486,35 @@
     <t>Topic: name- Week 10, lectures- 2 Lectures, duration- 01:19;
 Video: link- https://drive.google.com/file/d/1hrYmZgBA3wWiNbPf_0y_EjNAqVAep68S/preview, name- SRE Week # 10 Part 1.mp4, duration- 00:47;
 Video: link- https://drive.google.com/file/d/1C04hEIeBg2hEUmLco-5QQbT3AWkTYPIz/preview, name- SRE Week # 10 Part 2.mp4, duration- 00:32;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 12, lectures- 2 Lectures, duration- 01:36;
+Video: link- https://drive.google.com/file/d/1kOuhYo1poWvPz8T0eoBRzsXcoKoY7U12/preview, name- AD&amp;AA Week # 12 Part 1.mp4, duration- 00:58;
+Video: link- https://drive.google.com/file/d/1t2dXItzIgFA2pX8ZnqEudZNZBvRmACIF/preview, name- AD&amp;AA Week # 12 Part 2.mp4, duration- 00:38;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 9, lectures- 1 Lecture, duration- 01:18;
+Video: link- https://drive.google.com/file/d/13wRNzU6PSClUQ2hdxH6xlae5zPEjHR2d/preview, name- TPL Week # 9.mp4, duration- 01:18;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 11, lectures- 2 Lectures, duration- 00:56;
+Video: link- https://drive.google.com/file/d/1iGjE5XenE92z_rJ_1-lJD1LYZIY4clXC/preview, name- SRE Week # 11 Part 1.mp4, duration- 00:42;
+Video: link- https://drive.google.com/file/d/1lM0So4usTGuTnFKxlFqhn04Cv3P0bVqP/preview, name- SRE Week # 11 Part 2.mp4, duration- 00:14;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 12, lectures- Not uploaded, duration- -;
+Note: heading- Lectures not uploaded yet;</t>
+  </si>
+  <si>
+    <t>Topic: name- Final Term Exam, lectures- , duration- 27 Dec | 16:00-17:30;
+Assignment: name- Presentations List, link- presentation list.xlsx;
+Slides: slide- lec5.ppt;
+Slides: slide- Lec6.pptx;
+Slides: slide- lec7.pptx;
+Slides: slide- lec8.pdf;
+Slides: slide- lec9.pptx;
+Slides: slide- lec10.pdf;
+Note: heading- Syllabus not final yet. But these lectures are taught after mids;</t>
   </si>
 </sst>
 </file>
@@ -910,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB8366-CFB7-BD41-BAF1-2BC53FC93C19}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1115,7 +1136,7 @@
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="14" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>61</v>
@@ -1131,7 +1152,7 @@
         <v>66</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E13" s="14" t="s">
         <v>62</v>
@@ -1141,28 +1162,36 @@
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E14" s="14" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="170" x14ac:dyDescent="0.2">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C15" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="204" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="11"/>
+      <c r="E16" s="14" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="8"/>

</xml_diff>

<commit_message>
folders placed for other subjects also
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/QasimAli/nodejs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB1614F-1A58-8140-B755-573824946309}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6EB1D2-1F64-DF4F-903D-7490C07253B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="18580" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="76">
   <si>
     <t>Algo</t>
   </si>
@@ -506,15 +506,24 @@
 Note: heading- Lectures not uploaded yet;</t>
   </si>
   <si>
-    <t>Topic: name- Final Term Exam, lectures- , duration- 27 Dec | 16:00-17:30;
-Assignment: name- Presentations List, link- presentation list.xlsx;
+    <t>Topic: name- Final Term Exam, lectures- , duration- 30 Dec | 15:00-17:00;
+Note: heading- Being sorted. please visit later.;</t>
+  </si>
+  <si>
+    <t>Topic: name- Final Term Exam, lectures- , duration- 29 Dec | 12:30-14:30;
+Note: heading- Being sorted. please visit later.;</t>
+  </si>
+  <si>
+    <t>Topic: name- Final Term Exam, lectures- , duration- 27 Dec | 15:00-17:00;
+Assignment: name- presentation list.xlsx, link- presentation list.xlsx;
+Slides: slide- lec4.pptx;
 Slides: slide- lec5.ppt;
 Slides: slide- Lec6.pptx;
 Slides: slide- lec7.pptx;
 Slides: slide- lec8.pdf;
 Slides: slide- lec9.pptx;
 Slides: slide- lec10.pdf;
-Note: heading- Syllabus not final yet. But these lectures are taught after mids;</t>
+Note: heading- Syllabus not final yet. But these lectures are taught after mids.;</t>
   </si>
 </sst>
 </file>
@@ -1184,13 +1193,17 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="204" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="221" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
+      <c r="C16" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>74</v>
+      </c>
       <c r="E16" s="14" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added papers for algo
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/QasimAli/nodejs/renovationUpdates/server/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6EB1D2-1F64-DF4F-903D-7490C07253B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67ED6CA7-F4CC-1946-B616-DC0175C0F56E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="18580" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16700" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -515,15 +515,14 @@
   </si>
   <si>
     <t>Topic: name- Final Term Exam, lectures- , duration- 27 Dec | 15:00-17:00;
-Assignment: name- presentation list.xlsx, link- presentation list.xlsx;
-Slides: slide- lec4.pptx;
+Assignment: name- presentation list.xlsx, link- presentation list.xlsx;Assignment: name- Group 2 paper.pdf, link- Group 2 paper.pdf;
+Assignment: name- Group 2 presentation.pptx, link- Group 2 presentation.pptx;
+Assignment: name- Group 8 paper.pdf, link- Group 8 paper.pdf;
 Slides: slide- lec5.ppt;
 Slides: slide- Lec6.pptx;
-Slides: slide- lec7.pptx;
 Slides: slide- lec8.pdf;
 Slides: slide- lec9.pptx;
-Slides: slide- lec10.pdf;
-Note: heading- Syllabus not final yet. But these lectures are taught after mids.;</t>
+Note: heading- Syllabus is final. 1 question will come from Group 2 paper and Group 8 paer (attached above).;</t>
   </si>
 </sst>
 </file>
@@ -940,7 +939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB8366-CFB7-BD41-BAF1-2BC53FC93C19}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D15" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -1193,7 +1192,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="221" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="255" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="14" t="s">

</xml_diff>

<commit_message>
added topics for week 10
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/QasimAli/nodejs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6EB1D2-1F64-DF4F-903D-7490C07253B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3D7B57-5F63-9749-A1AE-03E38502F60A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="18580" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
@@ -450,12 +450,6 @@
 Slides: slide- Lecture Slide_5.pptx;</t>
   </si>
   <si>
-    <t>Topic: name- Week 10, lectures- 2 Lectures, duration- 01:24;
-Video: link- https://drive.google.com/file/d/1dy930AUWj6FhpQW_GAbGijpuZLD7owMZ/preview, name- AD&amp;AA Week # 10 Part 1.mp4, duration- 00:54;
-Video: link- https://drive.google.com/file/d/1Yz6n4GBQL6TryaLlmySsDhCP9y4XplkR/preview, name- AD&amp;AA Week # 10 Part 2.mp4, duration- 00:30;
-Slides: slide- Lec6.pptx;</t>
-  </si>
-  <si>
     <t>Topic: name- Week 11, lectures- 2 Lectures, duration- 01:18;
 Video: link- https://drive.google.com/file/d/1L8AXlWHcUH16jcl_Zu8UyUj6iwnvuCx-/preview, name- AD&amp;AA Week # 11 Part 1.mp4, duration- 00:52;
 Video: link- https://drive.google.com/file/d/1ba5ptKIgEeli77GEPoVeP-v6XeBzV_nU/preview, name- AD&amp;AA Week # 11 Part 2.mp4, duration- 00:26;
@@ -524,6 +518,13 @@
 Slides: slide- lec9.pptx;
 Slides: slide- lec10.pdf;
 Note: heading- Syllabus not final yet. But these lectures are taught after mids.;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 10, lectures- 2 Lectures, duration- 01:24;
+Video: link- https://drive.google.com/file/d/1dy930AUWj6FhpQW_GAbGijpuZLD7owMZ/preview, name- AD&amp;AA Week # 10 Part 1.mp4, duration- 00:54;
+Video: link- https://drive.google.com/file/d/1Yz6n4GBQL6TryaLlmySsDhCP9y4XplkR/preview, name- AD&amp;AA Week # 10 Part 2.mp4, duration- 00:30;
+Slides: slide- Lec6.pptx;
+Topics: Chapter 6, P NP &amp; NPC Computing problems, Vortex Cover Problem, Subset Sum Problem;</t>
   </si>
 </sst>
 </file>
@@ -940,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB8366-CFB7-BD41-BAF1-2BC53FC93C19}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1119,7 +1120,7 @@
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>55</v>
@@ -1132,7 +1133,7 @@
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>57</v>
@@ -1145,7 +1146,7 @@
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>61</v>
@@ -1154,56 +1155,56 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="187" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="221" x14ac:dyDescent="0.2">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="204" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="170" x14ac:dyDescent="0.2">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="221" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="E16" s="14" t="s">
         <v>74</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added topics till week 12 half
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/QasimAli/nodejs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3D7B57-5F63-9749-A1AE-03E38502F60A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F94725-BBE3-9D43-AE7D-11C018FDF7ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="18580" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="21640" windowHeight="20080" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -450,12 +450,6 @@
 Slides: slide- Lecture Slide_5.pptx;</t>
   </si>
   <si>
-    <t>Topic: name- Week 11, lectures- 2 Lectures, duration- 01:18;
-Video: link- https://drive.google.com/file/d/1L8AXlWHcUH16jcl_Zu8UyUj6iwnvuCx-/preview, name- AD&amp;AA Week # 11 Part 1.mp4, duration- 00:52;
-Video: link- https://drive.google.com/file/d/1ba5ptKIgEeli77GEPoVeP-v6XeBzV_nU/preview, name- AD&amp;AA Week # 11 Part 2.mp4, duration- 00:26;
-Assignment: name- Assignment 4, img- /ALGO/Assignment 4.png;</t>
-  </si>
-  <si>
     <t>Topic: name- Week 8, lectures- 1 Lecture, duration- 01:26;
 Video: link- https://drive.google.com/file/d/1Uc4upqacrhA2-FtxU8GKFDuNC_Mw8Pmz/preview, name- TPL Week # 8.mp4, duration- 01:26;
 Slides: slide- Chapter 6.ppt;
@@ -482,11 +476,6 @@
 Video: link- https://drive.google.com/file/d/1C04hEIeBg2hEUmLco-5QQbT3AWkTYPIz/preview, name- SRE Week # 10 Part 2.mp4, duration- 00:32;</t>
   </si>
   <si>
-    <t>Topic: name- Week 12, lectures- 2 Lectures, duration- 01:36;
-Video: link- https://drive.google.com/file/d/1kOuhYo1poWvPz8T0eoBRzsXcoKoY7U12/preview, name- AD&amp;AA Week # 12 Part 1.mp4, duration- 00:58;
-Video: link- https://drive.google.com/file/d/1t2dXItzIgFA2pX8ZnqEudZNZBvRmACIF/preview, name- AD&amp;AA Week # 12 Part 2.mp4, duration- 00:38;</t>
-  </si>
-  <si>
     <t>Topic: name- Week 9, lectures- 1 Lecture, duration- 01:18;
 Video: link- https://drive.google.com/file/d/13wRNzU6PSClUQ2hdxH6xlae5zPEjHR2d/preview, name- TPL Week # 9.mp4, duration- 01:18;</t>
   </si>
@@ -506,18 +495,6 @@
   <si>
     <t>Topic: name- Final Term Exam, lectures- , duration- 29 Dec | 12:30-14:30;
 Note: heading- Being sorted. please visit later.;</t>
-  </si>
-  <si>
-    <t>Topic: name- Final Term Exam, lectures- , duration- 27 Dec | 15:00-17:00;
-Assignment: name- presentation list.xlsx, link- presentation list.xlsx;
-Slides: slide- lec4.pptx;
-Slides: slide- lec5.ppt;
-Slides: slide- Lec6.pptx;
-Slides: slide- lec7.pptx;
-Slides: slide- lec8.pdf;
-Slides: slide- lec9.pptx;
-Slides: slide- lec10.pdf;
-Note: heading- Syllabus not final yet. But these lectures are taught after mids.;</t>
   </si>
   <si>
     <t>Topic: name- Week 10, lectures- 2 Lectures, duration- 01:24;
@@ -525,6 +502,31 @@
 Video: link- https://drive.google.com/file/d/1Yz6n4GBQL6TryaLlmySsDhCP9y4XplkR/preview, name- AD&amp;AA Week # 10 Part 2.mp4, duration- 00:30;
 Slides: slide- Lec6.pptx;
 Topics: Chapter 6, P NP &amp; NPC Computing problems, Vortex Cover Problem, Subset Sum Problem;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 11, lectures- 2 Lectures, duration- 01:18;
+Video: link- https://drive.google.com/file/d/1L8AXlWHcUH16jcl_Zu8UyUj6iwnvuCx-/preview, name- AD&amp;AA Week # 11 Part 1.mp4, duration- 00:52;
+Video: link- https://drive.google.com/file/d/1ba5ptKIgEeli77GEPoVeP-v6XeBzV_nU/preview, name- AD&amp;AA Week # 11 Part 2.mp4, duration- 00:26;
+Assignment: name- Assignment 4, img- /ALGO/Assignment 4.png;
+Topics: Word length optimization, Chapter 7 started;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 12, lectures- 2 Lectures, duration- 01:36;
+Video: link- https://drive.google.com/file/d/1kOuhYo1poWvPz8T0eoBRzsXcoKoY7U12/preview, name- AD&amp;AA Week # 12 Part 1.mp4, duration- 00:58;
+Video: link- https://drive.google.com/file/d/1t2dXItzIgFA2pX8ZnqEudZNZBvRmACIF/preview, name- AD&amp;AA Week # 12 Part 2.mp4, duration- 00:38;
+Topics: Chapter 7 Continued, Chapter 8, Arrays, Trees, Height Depth &amp; Level of Trees, Chapter 9, Stack, RPN;</t>
+  </si>
+  <si>
+    <t>Topic: name- Final Term Exam, lectures- , duration- 27 Dec | 15:00-17:00;
+Assignment: name- presentation list.xlsx, link- presentation list.xlsx;
+Assignment: name- Group 2 paper.pdf, link- Group 2 paper.pdf;
+Assignment: name- Group 2 presentation.pptx, link- Group 2 presentation.pptx;
+Assignment: name- Group 8 paper.pdf, link- Group 8 paper.pdf;
+Slides: slide- lec5.ppt;
+Slides: slide- Lec6.pptx;
+Slides: slide- lec8.pdf;
+Slides: slide- lec9.pptx;
+Note: heading- Syllabus is final. 1 question will come from Group 2 paper and Group 8 paper (attached above).</t>
   </si>
 </sst>
 </file>
@@ -941,8 +943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB8366-CFB7-BD41-BAF1-2BC53FC93C19}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="C14" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1120,7 +1122,7 @@
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>55</v>
@@ -1133,7 +1135,7 @@
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>57</v>
@@ -1146,7 +1148,7 @@
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>61</v>
@@ -1159,52 +1161,52 @@
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="204" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="221" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="170" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="204" x14ac:dyDescent="0.2">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="221" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="272" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
All Courses uploaded for finals
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/QasimAli/nodejs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F94725-BBE3-9D43-AE7D-11C018FDF7ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938DC046-EA02-FB4D-BC7D-73E2256A2515}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="21640" windowHeight="20080" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
@@ -489,14 +489,6 @@
 Note: heading- Lectures not uploaded yet;</t>
   </si>
   <si>
-    <t>Topic: name- Final Term Exam, lectures- , duration- 30 Dec | 15:00-17:00;
-Note: heading- Being sorted. please visit later.;</t>
-  </si>
-  <si>
-    <t>Topic: name- Final Term Exam, lectures- , duration- 29 Dec | 12:30-14:30;
-Note: heading- Being sorted. please visit later.;</t>
-  </si>
-  <si>
     <t>Topic: name- Week 10, lectures- 2 Lectures, duration- 01:24;
 Video: link- https://drive.google.com/file/d/1dy930AUWj6FhpQW_GAbGijpuZLD7owMZ/preview, name- AD&amp;AA Week # 10 Part 1.mp4, duration- 00:54;
 Video: link- https://drive.google.com/file/d/1Yz6n4GBQL6TryaLlmySsDhCP9y4XplkR/preview, name- AD&amp;AA Week # 10 Part 2.mp4, duration- 00:30;
@@ -527,6 +519,29 @@
 Slides: slide- lec8.pdf;
 Slides: slide- lec9.pptx;
 Note: heading- Syllabus is final. 1 question will come from Group 2 paper and Group 8 paper (attached above).</t>
+  </si>
+  <si>
+    <t>Topic: name- Final Term Exam, lectures- , duration- 29 Dec | 12:30-14:30;
+Slides: slide- Lecture Slide_2.pptx;
+Slides: slide- Lecture Slide_3.pptx;
+Slides: slide- Lecture Slide_4.pptx;
+Slides: slide- Lecture Slide_5.pptx;
+Slides: slide- Lecture Slide_6.pptx;
+Slides: slide- Lecture Slide_7.pptx;
+Note: heading- Lecture 2 to 4 were taught before mids are also included in Finals.;</t>
+  </si>
+  <si>
+    <t>Topic: name- Final Term Exam, lectures- , duration- 30 Dec | 1500-1700;
+Slides: slide- Chapter 1.ppt;
+Slides: slide- Chapter 2.ppt;
+Slides: slide- Chapter 3.ppt;
+Slides: slide- Chapter 4.ppt;
+Slides: slide- Chapter 5.pptx;
+Slides: slide- Chapter 6.ppt;
+Slides: slide- Chapter 7.ppt;
+Books: name- Chapter 8.ppt;
+Books: name- Chapter 9.ppt;
+Note: heading- Chapter 8 and 9 not uploaded yet. Chapter 1 to 5 were taught before mids are also included for finals;</t>
   </si>
 </sst>
 </file>
@@ -943,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB8366-CFB7-BD41-BAF1-2BC53FC93C19}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C14" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -999,7 +1014,7 @@
       <c r="G2" s="12"/>
       <c r="N2" s="6"/>
     </row>
-    <row r="3" spans="1:14" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>43720</v>
       </c>
@@ -1167,7 +1182,7 @@
         <v>66</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="221" x14ac:dyDescent="0.2">
@@ -1180,7 +1195,7 @@
         <v>68</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="204" x14ac:dyDescent="0.2">
@@ -1193,27 +1208,26 @@
         <v>69</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="272" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="14" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
+      <c r="D17" s="14"/>
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
past paper added for algo
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/QasimAli/nodejs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{938DC046-EA02-FB4D-BC7D-73E2256A2515}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50EBBAC6-1B76-6A44-A611-EB79CE8FE835}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="21640" windowHeight="20080" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
@@ -509,18 +509,6 @@
 Topics: Chapter 7 Continued, Chapter 8, Arrays, Trees, Height Depth &amp; Level of Trees, Chapter 9, Stack, RPN;</t>
   </si>
   <si>
-    <t>Topic: name- Final Term Exam, lectures- , duration- 27 Dec | 15:00-17:00;
-Assignment: name- presentation list.xlsx, link- presentation list.xlsx;
-Assignment: name- Group 2 paper.pdf, link- Group 2 paper.pdf;
-Assignment: name- Group 2 presentation.pptx, link- Group 2 presentation.pptx;
-Assignment: name- Group 8 paper.pdf, link- Group 8 paper.pdf;
-Slides: slide- lec5.ppt;
-Slides: slide- Lec6.pptx;
-Slides: slide- lec8.pdf;
-Slides: slide- lec9.pptx;
-Note: heading- Syllabus is final. 1 question will come from Group 2 paper and Group 8 paper (attached above).</t>
-  </si>
-  <si>
     <t>Topic: name- Final Term Exam, lectures- , duration- 29 Dec | 12:30-14:30;
 Slides: slide- Lecture Slide_2.pptx;
 Slides: slide- Lecture Slide_3.pptx;
@@ -542,6 +530,19 @@
 Books: name- Chapter 8.ppt;
 Books: name- Chapter 9.ppt;
 Note: heading- Chapter 8 and 9 not uploaded yet. Chapter 1 to 5 were taught before mids are also included for finals;</t>
+  </si>
+  <si>
+    <t>Topic: name- Final Term Exam, lectures- , duration- 27 Dec | 15:00-17:00;
+Assignment: name- presentation list.xlsx, link- presentation list.xlsx;
+Assignment: name- Group 2 paper.pdf, link- Group 2 paper.pdf;
+Assignment: name- Group 2 presentation.pptx, link- Group 2 presentation.pptx;
+Assignment: name- Group 8 paper.pdf, link- Group 8 paper.pdf;
+Slides: slide- lec5.ppt;
+Slides: slide- Lec6.pptx;
+Slides: slide- lec8.pdf;
+Slides: slide- lec9.pptx;
+Assignment: name- Past paper 2018 (2 photos), img- /ALGO/Past paper page 1.jpeg*/ALGO/Past paper page 2.jpeg;
+Note: heading- Syllabus is final. 1 question will come from Group 2 paper and Group 8 paper (attached above).</t>
   </si>
 </sst>
 </file>
@@ -958,8 +959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB8366-CFB7-BD41-BAF1-2BC53FC93C19}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1014,7 +1015,7 @@
       <c r="G2" s="12"/>
       <c r="N2" s="6"/>
     </row>
-    <row r="3" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>43720</v>
       </c>
@@ -1211,17 +1212,17 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="272" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="323" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="14" t="s">
         <v>75</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added chapter 8 for tpl
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/QasimAli/nodejs/renovationUpdates/server/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50EBBAC6-1B76-6A44-A611-EB79CE8FE835}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E664D0E-F665-CB49-A5F5-0B68E70CDAFA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21640" windowHeight="20080" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="21640" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -509,29 +509,6 @@
 Topics: Chapter 7 Continued, Chapter 8, Arrays, Trees, Height Depth &amp; Level of Trees, Chapter 9, Stack, RPN;</t>
   </si>
   <si>
-    <t>Topic: name- Final Term Exam, lectures- , duration- 29 Dec | 12:30-14:30;
-Slides: slide- Lecture Slide_2.pptx;
-Slides: slide- Lecture Slide_3.pptx;
-Slides: slide- Lecture Slide_4.pptx;
-Slides: slide- Lecture Slide_5.pptx;
-Slides: slide- Lecture Slide_6.pptx;
-Slides: slide- Lecture Slide_7.pptx;
-Note: heading- Lecture 2 to 4 were taught before mids are also included in Finals.;</t>
-  </si>
-  <si>
-    <t>Topic: name- Final Term Exam, lectures- , duration- 30 Dec | 1500-1700;
-Slides: slide- Chapter 1.ppt;
-Slides: slide- Chapter 2.ppt;
-Slides: slide- Chapter 3.ppt;
-Slides: slide- Chapter 4.ppt;
-Slides: slide- Chapter 5.pptx;
-Slides: slide- Chapter 6.ppt;
-Slides: slide- Chapter 7.ppt;
-Books: name- Chapter 8.ppt;
-Books: name- Chapter 9.ppt;
-Note: heading- Chapter 8 and 9 not uploaded yet. Chapter 1 to 5 were taught before mids are also included for finals;</t>
-  </si>
-  <si>
     <t>Topic: name- Final Term Exam, lectures- , duration- 27 Dec | 15:00-17:00;
 Assignment: name- presentation list.xlsx, link- presentation list.xlsx;
 Assignment: name- Group 2 paper.pdf, link- Group 2 paper.pdf;
@@ -543,6 +520,28 @@
 Slides: slide- lec9.pptx;
 Assignment: name- Past paper 2018 (2 photos), img- /ALGO/Past paper page 1.jpeg*/ALGO/Past paper page 2.jpeg;
 Note: heading- Syllabus is final. 1 question will come from Group 2 paper and Group 8 paper (attached above).</t>
+  </si>
+  <si>
+    <t>Topic: name- Final Term Exam, lectures- , duration- 29 Dec | 12:30-14:30;
+Slides: slide- Lecture Slide_2.pptx;
+Slides: slide- Lecture Slide_3.pptx;
+Slides: slide- Lecture Slide_4.pptx;
+Slides: slide- Lecture Slide_5.pptx;
+Slides: slide- Lecture Slide_6.pptx;
+Slides: slide- Lecture Slide_7.pptx;
+Note: heading- Syllabus is final. Lecture 2 to 4 were taught before mids are also included in Finals.;</t>
+  </si>
+  <si>
+    <t>Topic: name- Final Term Exam, lectures- , duration- 30 Dec | 1500-1700;
+Slides: slide- Chapter 1.ppt;
+Slides: slide- Chapter 2.ppt;
+Slides: slide- Chapter 3.ppt;
+Slides: slide- Chapter 4.ppt;
+Slides: slide- Chapter 5.pptx;
+Slides: slide- Chapter 6.ppt;
+Slides: slide- Chapter 7.ppt;
+Slides: slide- Chapter 8.pptx;
+Note: heading- Sullabus is final. Chapter 1 to 5 were taught before mids are also included for finals.;</t>
   </si>
 </sst>
 </file>
@@ -960,7 +959,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1216,13 +1215,13 @@
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="E16" s="14" t="s">
         <v>73</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fixed links to assignments for algo
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/QasimAli/nodejs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50EBBAC6-1B76-6A44-A611-EB79CE8FE835}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A0D030E-A884-794D-89F4-E4E0665E2C79}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21640" windowHeight="20080" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
+    <workbookView xWindow="6900" yWindow="4860" windowWidth="21640" windowHeight="20080" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -241,17 +241,6 @@
 Topics: Knuth Morris Algorithum, Boyer Moore Algorithum, Algorithum time comparison;</t>
   </si>
   <si>
-    <t>Topic: name- Week 1,lectures- 4 Lectures, duration- 01:38;
-Video: link- https://drive.google.com/file/d/1rba7mKiAH4UScARCW3HuCe5_LsdgofF_/preview, name- Class CR Number, duration- 00:00;
-Video: link- https://drive.google.com/file/d/1EvOHehNqZlji9HeyW6YYI6pGN-apUz8D/preview, name- AD&amp;AA Week#1 Part1.mp4, duration- 00:58;
-Video: link- https://drive.google.com/file/d/1PQ9EuYIsfZiHfxVupjg5JThWLEUT-1ka/preview, name- AD&amp;AA Week#1 Part2.mp4, duration- 00:32;
-Video: link- https://drive.google.com/file/d/1RfT5B3ulAR_QIrI8ktEg9r5u-FHZFxa3/preview, name- AD&amp;AA Week#1 Part3.mp4, duration- 00:14;
-Slides: slide- lec1.pptx;
-Assignment: name- Assignment # 1 Summary of Cincinati Website , link- /ALGO/cincinati.png;
-Assignment: name- Assignment # 2 Load Bty 18650 Algorithum , link- /ALGO/18650.png;
-Topics: Definition of Algorithum, Types of Algorithums, Flow Diagram Symbols, e la russ algorithum, Divide and COnquor algorithum, Parameters for selection of algorithum, e la russ algorithum if statements;</t>
-  </si>
-  <si>
     <t>Subject: Advance Theory and Design of Algorithum;
 Instructor: Dr Aqib Perwaiz;
 ClassSenior: Jasim, +92 323 4154345;
@@ -543,6 +532,17 @@
 Slides: slide- lec9.pptx;
 Assignment: name- Past paper 2018 (2 photos), img- /ALGO/Past paper page 1.jpeg*/ALGO/Past paper page 2.jpeg;
 Note: heading- Syllabus is final. 1 question will come from Group 2 paper and Group 8 paper (attached above).</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 1,lectures- 4 Lectures, duration- 01:38;
+Video: link- https://drive.google.com/file/d/1rba7mKiAH4UScARCW3HuCe5_LsdgofF_/preview, name- Class CR Number, duration- 00:00;
+Video: link- https://drive.google.com/file/d/1EvOHehNqZlji9HeyW6YYI6pGN-apUz8D/preview, name- AD&amp;AA Week#1 Part1.mp4, duration- 00:58;
+Video: link- https://drive.google.com/file/d/1PQ9EuYIsfZiHfxVupjg5JThWLEUT-1ka/preview, name- AD&amp;AA Week#1 Part2.mp4, duration- 00:32;
+Video: link- https://drive.google.com/file/d/1RfT5B3ulAR_QIrI8ktEg9r5u-FHZFxa3/preview, name- AD&amp;AA Week#1 Part3.mp4, duration- 00:14;
+Slides: slide- lec1.pptx;
+Assignment: name- Assignment # 1 Summary of Cincinati Website , img- /ALGO/cincinati.png;
+Assignment: name- Assignment # 2 Load Bty 18650 Algorithum , img- /ALGO/18650.png;
+Topics: Definition of Algorithum, Types of Algorithums, Flow Diagram Symbols, e la russ algorithum, Divide and COnquor algorithum, Parameters for selection of algorithum, e la russ algorithum if statements;</t>
   </si>
 </sst>
 </file>
@@ -959,8 +959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB8366-CFB7-BD41-BAF1-2BC53FC93C19}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -990,7 +990,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G1" s="12"/>
       <c r="N1" s="6"/>
@@ -1001,36 +1001,36 @@
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G2" s="12"/>
       <c r="N2" s="6"/>
     </row>
-    <row r="3" spans="1:14" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>43720</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G3" s="12"/>
       <c r="N3" s="6"/>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>29</v>
@@ -1059,10 +1059,10 @@
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>32</v>
@@ -1075,7 +1075,7 @@
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>31</v>
@@ -1091,13 +1091,13 @@
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
@@ -1109,13 +1109,13 @@
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F8" s="10"/>
     </row>
@@ -1125,104 +1125,104 @@
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="14" t="s">
-        <v>47</v>
-      </c>
       <c r="E9" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="238" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="306" x14ac:dyDescent="0.2">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D11" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="14" t="s">
         <v>57</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="323" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="221" x14ac:dyDescent="0.2">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="221" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="204" x14ac:dyDescent="0.2">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="323" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" s="14" t="s">
         <v>74</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated week 12 for tpl and sre
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/QasimAli/nodejs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08033D5-FD32-4644-9867-A678D1855660}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12BE0767-DA0D-E443-85F7-59567F69E93B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21640" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
+    <workbookView xWindow="22740" yWindow="8420" windowWidth="21640" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="77">
   <si>
     <t>Algo</t>
   </si>
@@ -450,22 +450,12 @@
 Slides: slide- Lecture Slide_5.pptx;</t>
   </si>
   <si>
-    <t>Topic: name- Week 8, lectures- 1 Lecture, duration- 01:26;
-Video: link- https://drive.google.com/file/d/1Uc4upqacrhA2-FtxU8GKFDuNC_Mw8Pmz/preview, name- TPL Week # 8.mp4, duration- 01:26;
-Slides: slide- Chapter 6.ppt;
-Assignment: name- Assignment no 3 (Deadline 15 Dec 2019), img- /TPL/Assignment No 3 TPL.png;</t>
-  </si>
-  <si>
     <t>Topic: name- Week 7, lectures- Assignment Only, duration- -;
 Assignment: name- Assignment no 2 (Deadline 23 Nov), img- /TPL/Assignment2.jpeg*/TPL/mid20191.jpg*/TPL/mid20192.jpg;
 Assignment: name- Assignment no 2 Solved, link- Assignment 2 Solved.docx;
 Note: heading- Note, text- No lecture conducted during this week due to exam on 17 Nov 2019. Sir only gave above assignment.;</t>
   </si>
   <si>
-    <t>Topic: name- Week 10, lectures- Not uploaded, duration- -;
-Note: heading- Lectures not uploaded yet;</t>
-  </si>
-  <si>
     <t>Topic: name- Week 11, lectures- Assignment Only, duration- -;
 Slides: slide- Chapter 7.ppt;
 Assignment: name- Quiz in next class from above Chapter 7, img- /TPL/Assignment 4.png;</t>
@@ -474,10 +464,6 @@
     <t>Topic: name- Week 10, lectures- 2 Lectures, duration- 01:19;
 Video: link- https://drive.google.com/file/d/1hrYmZgBA3wWiNbPf_0y_EjNAqVAep68S/preview, name- SRE Week # 10 Part 1.mp4, duration- 00:47;
 Video: link- https://drive.google.com/file/d/1C04hEIeBg2hEUmLco-5QQbT3AWkTYPIz/preview, name- SRE Week # 10 Part 2.mp4, duration- 00:32;</t>
-  </si>
-  <si>
-    <t>Topic: name- Week 9, lectures- 1 Lecture, duration- 01:18;
-Video: link- https://drive.google.com/file/d/13wRNzU6PSClUQ2hdxH6xlae5zPEjHR2d/preview, name- TPL Week # 9.mp4, duration- 01:18;</t>
   </si>
   <si>
     <t>Topic: name- Week 11, lectures- 2 Lectures, duration- 00:56;
@@ -532,6 +518,16 @@
 Note: heading- Syllabus is final. Lecture 2 to 4 were taught before mids are also included in Finals.;</t>
   </si>
   <si>
+    <t>Topic: name- Week 9, lectures- 1 Lecture, duration- 01:18;
+Video: link- https://drive.google.com/file/d/13wRNzU6PSClUQ2hdxH6xlae5zPEjHR2d/preview, name- TPL Week # 9.mp4, duration- 01:18;
+Slides: slide- Chapter 8.pptx;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 10, lectures- 1 Lecture, duration- 01:06;
+Video: link- https://drive.google.com/file/d/12IYyBowEUKe90QhBUaHxXLSMomo1_aMj/preview, name- TPL Week # 10.mp4, duration- 01:06;
+Slides: slide- Chapter 9.ppt;</t>
+  </si>
+  <si>
     <t>Topic: name- Final Term Exam, lectures- , duration- 30 Dec | 1500-1700;
 Slides: slide- Chapter 3.ppt;
 Slides: slide- Chapter 4.ppt;
@@ -539,7 +535,18 @@
 Slides: slide- Chapter 6.ppt;
 Slides: slide- Chapter 7.ppt;
 Slides: slide- Chapter 8.pptx;
+Slides: slide- Chapter 9.ppt;
 Note: heading- Sullabus is final. Chapter 3 to 5 were taught before mids are also included for finals.;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 8, lectures- 1 Lecture, duration- 01:26;
+Video: link- https://drive.google.com/file/d/1Uc4upqacrhA2-FtxU8GKFDuNC_Mw8Pmz/preview, name- TPL Week # 8.mp4, duration- 01:26;
+Slides: slide- Chapter 7.ppt;
+Assignment: name- Assignment no 3 (Deadline 15 Dec 2019), img- /TPL/Assignment No 3 TPL.png;</t>
+  </si>
+  <si>
+    <t>Topic: name- Week 12, lectures- 1 Lecture, duration- 00:34;
+Video: link- https://drive.google.com/file/d/1OTYTl2ZxiHs7UH9LHHagN6WYGGONYMd2/preview, name- SRE Week # 11 Part 1.mp4, duration- 00:42;</t>
   </si>
 </sst>
 </file>
@@ -956,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB8366-CFB7-BD41-BAF1-2BC53FC93C19}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="C14" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1135,7 +1142,7 @@
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>55</v>
@@ -1148,7 +1155,7 @@
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="14" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>57</v>
@@ -1161,7 +1168,7 @@
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="14" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>61</v>
@@ -1174,52 +1181,52 @@
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="14" t="s">
-        <v>66</v>
-      </c>
       <c r="E13" s="14" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="221" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="E14" s="14" t="s">
         <v>68</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="204" x14ac:dyDescent="0.2">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="14" t="s">
         <v>69</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="323" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added solution to past paper
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/QasimAli/nodejs/renovationUpdates/server/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12BE0767-DA0D-E443-85F7-59567F69E93B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F11A91-019B-9A42-8EF5-C216BCD69E70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22740" yWindow="8420" windowWidth="21640" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -508,16 +508,6 @@
 Note: heading- Syllabus is final. 1 question will come from Group 2 paper and Group 8 paper (attached above).</t>
   </si>
   <si>
-    <t>Topic: name- Final Term Exam, lectures- , duration- 29 Dec | 12:30-14:30;
-Slides: slide- Lecture Slide_2.pptx;
-Slides: slide- Lecture Slide_3.pptx;
-Slides: slide- Lecture Slide_4.pptx;
-Slides: slide- Lecture Slide_5.pptx;
-Slides: slide- Lecture Slide_6.pptx;
-Slides: slide- Lecture Slide_7.pptx;
-Note: heading- Syllabus is final. Lecture 2 to 4 were taught before mids are also included in Finals.;</t>
-  </si>
-  <si>
     <t>Topic: name- Week 9, lectures- 1 Lecture, duration- 01:18;
 Video: link- https://drive.google.com/file/d/13wRNzU6PSClUQ2hdxH6xlae5zPEjHR2d/preview, name- TPL Week # 9.mp4, duration- 01:18;
 Slides: slide- Chapter 8.pptx;</t>
@@ -547,6 +537,19 @@
   <si>
     <t>Topic: name- Week 12, lectures- 1 Lecture, duration- 00:34;
 Video: link- https://drive.google.com/file/d/1OTYTl2ZxiHs7UH9LHHagN6WYGGONYMd2/preview, name- SRE Week # 11 Part 1.mp4, duration- 00:42;</t>
+  </si>
+  <si>
+    <t>Topic: name- Final Term Exam, lectures- , duration- 29 Dec | 12:30-14:30;
+Slides: slide- Lecture Slide_2.pptx;
+Slides: slide- Lecture Slide_3.pptx;
+Slides: slide- Lecture Slide_4.pptx;
+Slides: slide- Lecture Slide_5.pptx;
+Slides: slide- Lecture Slide_6.pptx;
+Slides: slide- Lecture Slide_7.pptx;
+Assignment: name- Past Paper Finals Fall 2017, img- /SRE/past paper 2017.jpg;
+Assignment: name- Solution of above paper, img- /SRE/past paper solved 1.png*/SRE/past paper solved 2.png*/SRE/past paper solved 3.png;
+Assignment: name- Solution of above paper in pdf, link- past paper 2017.pdf;
+Note: heading- Syllabus is final. Lecture 2 to 4 were taught before mids are also included in Finals.;</t>
   </si>
 </sst>
 </file>
@@ -963,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB8366-CFB7-BD41-BAF1-2BC53FC93C19}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C14" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1155,7 +1158,7 @@
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>57</v>
@@ -1168,7 +1171,7 @@
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>61</v>
@@ -1181,7 +1184,7 @@
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>64</v>
@@ -1210,7 +1213,7 @@
         <v>66</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E15" s="14" t="s">
         <v>69</v>
@@ -1220,10 +1223,10 @@
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="E16" s="14" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
past paper solution for tpl added
</commit_message>
<xml_diff>
--- a/server/life.xlsx
+++ b/server/life.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F11A91-019B-9A42-8EF5-C216BCD69E70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{501A411B-651E-CF40-BF62-74BCC0A61013}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{2E76D17A-07E1-904B-8BB7-AAF347409254}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -518,17 +518,6 @@
 Slides: slide- Chapter 9.ppt;</t>
   </si>
   <si>
-    <t>Topic: name- Final Term Exam, lectures- , duration- 30 Dec | 1500-1700;
-Slides: slide- Chapter 3.ppt;
-Slides: slide- Chapter 4.ppt;
-Slides: slide- Chapter 5.pptx;
-Slides: slide- Chapter 6.ppt;
-Slides: slide- Chapter 7.ppt;
-Slides: slide- Chapter 8.pptx;
-Slides: slide- Chapter 9.ppt;
-Note: heading- Sullabus is final. Chapter 3 to 5 were taught before mids are also included for finals.;</t>
-  </si>
-  <si>
     <t>Topic: name- Week 8, lectures- 1 Lecture, duration- 01:26;
 Video: link- https://drive.google.com/file/d/1Uc4upqacrhA2-FtxU8GKFDuNC_Mw8Pmz/preview, name- TPL Week # 8.mp4, duration- 01:26;
 Slides: slide- Chapter 7.ppt;
@@ -550,6 +539,19 @@
 Assignment: name- Solution of above paper, img- /SRE/past paper solved 1.png*/SRE/past paper solved 2.png*/SRE/past paper solved 3.png;
 Assignment: name- Solution of above paper in pdf, link- past paper 2017.pdf;
 Note: heading- Syllabus is final. Lecture 2 to 4 were taught before mids are also included in Finals.;</t>
+  </si>
+  <si>
+    <t>Topic: name- Final Term Exam, lectures- , duration- 30 Dec | 1500-1700;
+Slides: slide- Chapter 3.ppt;
+Slides: slide- Chapter 4.ppt;
+Slides: slide- Chapter 5.pptx;
+Slides: slide- Chapter 6.ppt;
+Slides: slide- Chapter 7.ppt;
+Slides: slide- Chapter 8.pptx;
+Slides: slide- Chapter 9.ppt;
+Assignment: name- Solution past paper (12 images), img- /TPL/past paper solved1.png*/TPL/past paper solved2.png*/TPL/past paper solved3.png*/TPL/past paper solved4.png*/TPL/past paper solved5.png*/TPL/past paper solved6.png*/TPL/past paper solved7.png*/TPL/past paper solved8.png*/TPL/past paper solved9.png*/TPL/past paper solved10.png*/TPL/past paper solved11.png*/TPL/past paper solved12.png;
+Assignment: name- Solution of above paper in pdf, link- TPL Solved Past Paper Finals Fall 2018.pdf;
+Note: heading- Sullabus is final. Chapter 3 to 5 were taught before mids are also included for finals.;</t>
   </si>
 </sst>
 </file>
@@ -967,7 +969,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1158,7 +1160,7 @@
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>57</v>
@@ -1213,20 +1215,20 @@
         <v>66</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E15" s="14" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="323" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="14" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E16" s="14" t="s">
         <v>70</v>

</xml_diff>